<commit_message>
[2018-10-30] Design document - update 1
</commit_message>
<xml_diff>
--- a/demo-design-doc/Feature List.xlsx
+++ b/demo-design-doc/Feature List.xlsx
@@ -3,15 +3,19 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A39BCD0-8093-434C-9AF1-6F4C3A12A751}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77D402E6-FD70-4564-BC00-82F4C4E6A81F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" tabRatio="707" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
     <sheet name="Customer Distribution" sheetId="3" r:id="rId2"/>
     <sheet name="Asset Management Overview" sheetId="4" r:id="rId3"/>
     <sheet name="Customer Trends Report" sheetId="6" r:id="rId4"/>
+    <sheet name="Customer Position" sheetId="7" r:id="rId5"/>
+    <sheet name="Share TXN Input" sheetId="8" r:id="rId6"/>
+    <sheet name="Connectivity" sheetId="10" r:id="rId7"/>
+    <sheet name="Sheet5" sheetId="11" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -23,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="147">
   <si>
     <t>Login</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -85,19 +89,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Share Input</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Quote Rate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Done</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>WIP</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -299,6 +291,332 @@
   <si>
     <t>Customer Overview
 &gt; Customer Trends Report</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Login : RM - Jack SMITH</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Trade Input</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Customer Number</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Customer Name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Total P&amp;L</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8000-123456</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nikko KITMAN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Oliver HUSIN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8000-677988</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8000-546700</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8000-544976</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8000-321456</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8000-698929</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ming Group LTD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Calvin ZUGBERG</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shawn BLIANCE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Kawasaki MIZUKA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Total Asset Value (USD)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Total Amount(USD)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Market Price</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Average Cost</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HSBC Holding</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Quantity</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P&amp;L(USD)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tencent</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Product Name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HSBC Bond 5Y</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CCY Pair</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HKD/USD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Buy Amout</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sell Amount</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bid/Offer Rate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Market Rate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Last Biz Date P&amp;L(USD)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Account Number</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Portfolio Summary</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Total Value</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Total P&amp;L Last Biz Date</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Trade Input
+&gt; Share Transaction Input</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Share Transaction Input</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Buy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sell</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Share Issue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Norminal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Share Price</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Trade Type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">eShare </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Phone</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Share Currency</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>House View</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Credit Rating</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Issue Name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Avg Price</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Holding Details</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0005.HK</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CCY</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Solicite </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Trade Input
+&gt; Connectivity</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Leg2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Leg 3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Leg 4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Leg1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Best Rate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BNP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Counter Party</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Share Issue Info</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Customer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Remark</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Last Closing Price</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8000-123456-0001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Limit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>For investment</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BULL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AA+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>N</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GB&amp;M</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Credit Swiss</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Morgan Stanley</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Connectivity</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -306,7 +624,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -354,8 +672,32 @@
       <name val="等线"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <name val="等线"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="等线"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -404,8 +746,38 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="14">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -548,12 +920,136 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="147">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
@@ -572,6 +1068,38 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -599,31 +1127,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -651,15 +1154,192 @@
     <xf numFmtId="0" fontId="4" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="4" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="17" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -771,6 +1451,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-E4BB-43A3-BE2F-2B74BC85FDDB}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -786,6 +1471,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-E4BB-43A3-BE2F-2B74BC85FDDB}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -801,6 +1491,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-E4BB-43A3-BE2F-2B74BC85FDDB}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -816,6 +1511,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-E4BB-43A3-BE2F-2B74BC85FDDB}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
@@ -4175,6 +4875,463 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>952500</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>838200</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="矩形 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E056EF04-D605-44E0-A17C-C0BD8C0CBD2F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4914900" y="1073150"/>
+          <a:ext cx="1943100" cy="234950"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>666750</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>69850</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="矩形: 圆角 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DE230263-7232-4DFA-B5F9-B909F3590BDD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7181850" y="1035050"/>
+          <a:ext cx="615950" cy="292100"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>Search</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>226785</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>1351642</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>145143</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="矩形: 圆角 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{211F86C6-AAFB-4EFA-A157-20C388012A59}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11901714" y="4717143"/>
+          <a:ext cx="1124857" cy="326571"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="1"/>
+            <a:t>Save As PDF</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>660081</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>99787</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>527744</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>52827</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="矩形: 圆角 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{22ACD339-5494-4ABB-8271-811B82420892}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7608795" y="3728358"/>
+          <a:ext cx="693163" cy="315898"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>Submit</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>90714</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>154214</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>81642</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="矩形: 圆角 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{387D0202-FC14-414D-854A-852FCFF1D40C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4726214" y="1605643"/>
+          <a:ext cx="2984500" cy="290285"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>Notes</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>426358</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>18143</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>780143</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>36286</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="箭头: 下 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5148B440-4ABA-49BA-96EB-E455B9039195}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7375072" y="1651000"/>
+          <a:ext cx="353785" cy="199572"/>
+        </a:xfrm>
+        <a:prstGeom prst="downArrow">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent4">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent4"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent4"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>689430</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>166006</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>553358</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="矩形: 圆角 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2F6141AD-3766-4AC9-95EF-6F65E25ECD1C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10713359" y="1617435"/>
+          <a:ext cx="943428" cy="323851"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="1"/>
+            <a:t>Quote</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100" b="1" baseline="0"/>
+            <a:t> Rate</a:t>
+          </a:r>
+          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -4440,8 +5597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -4456,10 +5613,10 @@
         <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -4476,8 +5633,8 @@
       <c r="D4" t="s">
         <v>2</v>
       </c>
-      <c r="E4" t="s">
-        <v>19</v>
+      <c r="E4" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="F4">
         <v>8</v>
@@ -4487,8 +5644,8 @@
       <c r="D5" t="s">
         <v>6</v>
       </c>
-      <c r="E5" t="s">
-        <v>19</v>
+      <c r="E5" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="F5">
         <v>9</v>
@@ -4500,11 +5657,11 @@
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="D7" s="51" t="s">
+      <c r="D7" s="33" t="s">
         <v>4</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F7">
         <v>1</v>
@@ -4514,8 +5671,8 @@
       <c r="D8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E8" t="s">
-        <v>19</v>
+      <c r="E8" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="F8">
         <v>3</v>
@@ -4531,7 +5688,7 @@
         <v>7</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F10">
         <v>2</v>
@@ -4552,7 +5709,7 @@
         <v>10</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F15">
         <v>7</v>
@@ -4564,11 +5721,11 @@
       </c>
     </row>
     <row r="17" spans="3:6">
-      <c r="D17" t="s">
+      <c r="D17" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F17">
         <v>4</v>
@@ -4580,22 +5737,22 @@
       </c>
     </row>
     <row r="19" spans="3:6">
-      <c r="D19" t="s">
+      <c r="D19" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="F19">
         <v>5</v>
       </c>
     </row>
     <row r="20" spans="3:6">
-      <c r="D20" t="s">
-        <v>16</v>
+      <c r="D20" s="2" t="s">
+        <v>146</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F20">
         <v>6</v>
@@ -4607,6 +5764,9 @@
     <hyperlink ref="D7" location="'Customer Distribution'!A1" display="Customer Distribution" xr:uid="{AF1C2B3B-A664-4357-8023-64D8386E1154}"/>
     <hyperlink ref="D10" location="'Asset Management Overview'!A1" display="Asset Management Overview" xr:uid="{6FCF5499-EE75-4A8F-9C92-6619A9480DEC}"/>
     <hyperlink ref="D8" location="'Customer Trends Report'!A1" display="Customer Trends Report" xr:uid="{339FDFF1-3ED0-4D6B-B25C-A6B3C22A655E}"/>
+    <hyperlink ref="D17" location="'Customer Position'!A1" display="Customer Position" xr:uid="{9CA30750-2810-40D7-AF82-1D30F0FC15EF}"/>
+    <hyperlink ref="D19" location="'Share TXN Input'!A1" display="Share Transaction Input" xr:uid="{39EB9BB3-56CE-41EE-AA9C-FC11AD553571}"/>
+    <hyperlink ref="D20" location="Connectivity!A1" display="Connectivity" xr:uid="{6656CEBB-CF00-47C7-A322-868A423C8EA9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4630,7 +5790,7 @@
     <row r="2" spans="4:14" ht="14.5" thickBot="1"/>
     <row r="3" spans="4:14">
       <c r="D3" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
@@ -4642,14 +5802,14 @@
         <v>0</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="M3" s="10"/>
       <c r="N3" s="11"/>
     </row>
     <row r="4" spans="4:14">
       <c r="D4" s="6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
@@ -4658,7 +5818,7 @@
       <c r="I4" s="7"/>
       <c r="J4" s="7"/>
       <c r="K4" s="7" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="L4" s="7"/>
       <c r="M4" s="12"/>
@@ -4678,22 +5838,22 @@
       <c r="N5" s="15"/>
     </row>
     <row r="6" spans="4:14">
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="E6" s="19"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="32" t="s">
+      <c r="E6" s="41"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="I6" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="J6" s="20" t="s">
         <v>26</v>
-      </c>
-      <c r="H6" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="I6" s="30" t="s">
-        <v>30</v>
-      </c>
-      <c r="J6" s="29" t="s">
-        <v>29</v>
       </c>
       <c r="K6" s="10"/>
       <c r="L6" s="10"/>
@@ -4701,17 +5861,17 @@
       <c r="N6" s="11"/>
     </row>
     <row r="7" spans="4:14">
-      <c r="D7" s="21"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="H7" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="I7" s="35" t="s">
-        <v>34</v>
+      <c r="D7" s="43"/>
+      <c r="E7" s="44"/>
+      <c r="F7" s="45"/>
+      <c r="G7" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="H7" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="I7" s="26" t="s">
+        <v>31</v>
       </c>
       <c r="J7" s="12"/>
       <c r="K7" s="12"/>
@@ -4720,49 +5880,49 @@
       <c r="N7" s="13"/>
     </row>
     <row r="8" spans="4:14" ht="14.5" thickBot="1">
-      <c r="D8" s="24"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="33" t="s">
-        <v>35</v>
+      <c r="D8" s="46"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="48"/>
+      <c r="G8" s="24" t="s">
+        <v>32</v>
       </c>
       <c r="H8" s="12"/>
-      <c r="I8" s="37" t="s">
-        <v>31</v>
-      </c>
-      <c r="J8" s="36" t="s">
-        <v>30</v>
-      </c>
-      <c r="K8" s="37" t="s">
-        <v>36</v>
+      <c r="I8" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="J8" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="K8" s="28" t="s">
+        <v>33</v>
       </c>
       <c r="L8" s="12"/>
       <c r="M8" s="12"/>
       <c r="N8" s="13"/>
     </row>
     <row r="9" spans="4:14">
-      <c r="D9" s="42" t="s">
+      <c r="D9" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="43"/>
-      <c r="F9" s="44"/>
-      <c r="G9" s="38" t="s">
-        <v>38</v>
-      </c>
-      <c r="H9" s="27"/>
-      <c r="I9" s="27"/>
-      <c r="J9" s="27"/>
-      <c r="K9" s="27"/>
-      <c r="L9" s="27"/>
-      <c r="M9" s="39">
+      <c r="E9" s="50"/>
+      <c r="F9" s="51"/>
+      <c r="G9" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="18"/>
+      <c r="M9" s="30">
         <v>100</v>
       </c>
-      <c r="N9" s="28"/>
+      <c r="N9" s="19"/>
     </row>
     <row r="10" spans="4:14">
-      <c r="D10" s="45"/>
-      <c r="E10" s="46"/>
-      <c r="F10" s="47"/>
+      <c r="D10" s="52"/>
+      <c r="E10" s="53"/>
+      <c r="F10" s="54"/>
       <c r="G10" s="12"/>
       <c r="H10" s="12"/>
       <c r="I10" s="12"/>
@@ -4773,9 +5933,9 @@
       <c r="N10" s="13"/>
     </row>
     <row r="11" spans="4:14">
-      <c r="D11" s="45"/>
-      <c r="E11" s="46"/>
-      <c r="F11" s="47"/>
+      <c r="D11" s="52"/>
+      <c r="E11" s="53"/>
+      <c r="F11" s="54"/>
       <c r="G11" s="12"/>
       <c r="H11" s="12"/>
       <c r="I11" s="12"/>
@@ -4786,35 +5946,35 @@
       <c r="N11" s="13"/>
     </row>
     <row r="12" spans="4:14" ht="14.5" thickBot="1">
-      <c r="D12" s="48"/>
-      <c r="E12" s="49"/>
-      <c r="F12" s="50"/>
+      <c r="D12" s="55"/>
+      <c r="E12" s="56"/>
+      <c r="F12" s="57"/>
       <c r="G12" s="12"/>
       <c r="H12" s="12"/>
       <c r="I12" s="12"/>
       <c r="J12" s="12"/>
       <c r="K12" s="12"/>
-      <c r="L12" s="40" t="s">
-        <v>26</v>
-      </c>
-      <c r="M12" s="40" t="s">
-        <v>41</v>
+      <c r="L12" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="M12" s="31" t="s">
+        <v>38</v>
       </c>
       <c r="N12" s="13"/>
     </row>
     <row r="13" spans="4:14">
-      <c r="D13" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="E13" s="19"/>
-      <c r="F13" s="20"/>
+      <c r="D13" s="40" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="41"/>
+      <c r="F13" s="42"/>
       <c r="G13" s="12"/>
       <c r="H13" s="12"/>
       <c r="I13" s="12"/>
       <c r="J13" s="12"/>
       <c r="K13" s="12"/>
       <c r="L13" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="M13" s="4">
         <v>9000</v>
@@ -4822,16 +5982,16 @@
       <c r="N13" s="13"/>
     </row>
     <row r="14" spans="4:14">
-      <c r="D14" s="21"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="23"/>
+      <c r="D14" s="43"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="45"/>
       <c r="G14" s="12"/>
       <c r="H14" s="12"/>
       <c r="I14" s="12"/>
       <c r="J14" s="12"/>
       <c r="K14" s="12"/>
       <c r="L14" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="M14" s="4">
         <v>4000</v>
@@ -4839,16 +5999,16 @@
       <c r="N14" s="13"/>
     </row>
     <row r="15" spans="4:14">
-      <c r="D15" s="21"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="23"/>
+      <c r="D15" s="43"/>
+      <c r="E15" s="44"/>
+      <c r="F15" s="45"/>
       <c r="G15" s="12"/>
       <c r="H15" s="12"/>
       <c r="I15" s="12"/>
       <c r="J15" s="12"/>
       <c r="K15" s="12"/>
       <c r="L15" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="M15" s="4">
         <v>1500</v>
@@ -4856,16 +6016,16 @@
       <c r="N15" s="13"/>
     </row>
     <row r="16" spans="4:14" ht="14.5" thickBot="1">
-      <c r="D16" s="24"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="26"/>
+      <c r="D16" s="46"/>
+      <c r="E16" s="47"/>
+      <c r="F16" s="48"/>
       <c r="G16" s="12"/>
       <c r="H16" s="12"/>
       <c r="I16" s="12"/>
       <c r="J16" s="12"/>
       <c r="K16" s="12"/>
       <c r="L16" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="M16" s="4">
         <v>500</v>
@@ -4881,10 +6041,10 @@
       <c r="I17" s="12"/>
       <c r="J17" s="12"/>
       <c r="K17" s="12"/>
-      <c r="L17" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="M17" s="41">
+      <c r="L17" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="M17" s="32">
         <f>SUM(M13:M16)</f>
         <v>15000</v>
       </c>
@@ -4946,7 +6106,7 @@
   <dimension ref="D2:N20"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:N20"/>
+      <selection activeCell="Q19" sqref="Q19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -4965,7 +6125,7 @@
     <row r="2" spans="4:14" ht="14.5" thickBot="1"/>
     <row r="3" spans="4:14">
       <c r="D3" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
@@ -4975,14 +6135,14 @@
       <c r="J3" s="5"/>
       <c r="K3" s="10"/>
       <c r="L3" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="M3" s="5"/>
       <c r="N3" s="11"/>
     </row>
     <row r="4" spans="4:14">
       <c r="D4" s="6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
@@ -4992,7 +6152,7 @@
       <c r="J4" s="7"/>
       <c r="K4" s="12"/>
       <c r="L4" s="7" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="M4" s="7"/>
       <c r="N4" s="13"/>
@@ -5011,103 +6171,103 @@
       <c r="N5" s="15"/>
     </row>
     <row r="6" spans="4:14">
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="E6" s="19"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="32" t="s">
-        <v>49</v>
-      </c>
-      <c r="H6" s="31" t="s">
-        <v>43</v>
-      </c>
-      <c r="I6" s="30" t="s">
+      <c r="E6" s="41"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="H6" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="I6" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="J6" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="K6" s="20"/>
+      <c r="L6" s="21" t="s">
         <v>44</v>
-      </c>
-      <c r="J6" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="K6" s="29"/>
-      <c r="L6" s="30" t="s">
-        <v>47</v>
       </c>
       <c r="M6" s="10"/>
       <c r="N6" s="11"/>
     </row>
     <row r="7" spans="4:14">
-      <c r="D7" s="21"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="33" t="s">
-        <v>26</v>
-      </c>
-      <c r="H7" s="34" t="s">
-        <v>31</v>
-      </c>
-      <c r="I7" s="35" t="s">
-        <v>30</v>
-      </c>
-      <c r="J7" s="34" t="s">
-        <v>50</v>
-      </c>
-      <c r="K7" s="34"/>
+      <c r="D7" s="43"/>
+      <c r="E7" s="44"/>
+      <c r="F7" s="45"/>
+      <c r="G7" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="I7" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="J7" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="K7" s="25"/>
       <c r="L7" s="12"/>
       <c r="M7" s="12"/>
       <c r="N7" s="13"/>
     </row>
     <row r="8" spans="4:14" ht="14.5" thickBot="1">
-      <c r="D8" s="24"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="33" t="s">
+      <c r="D8" s="46"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="48"/>
+      <c r="G8" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="H8" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="I8" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="J8" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="H8" s="35" t="s">
+      <c r="K8" s="28" t="s">
         <v>52</v>
-      </c>
-      <c r="I8" s="37" t="s">
-        <v>53</v>
-      </c>
-      <c r="J8" s="36" t="s">
-        <v>54</v>
-      </c>
-      <c r="K8" s="37" t="s">
-        <v>55</v>
       </c>
       <c r="L8" s="12"/>
       <c r="M8" s="12"/>
       <c r="N8" s="13"/>
     </row>
     <row r="9" spans="4:14">
-      <c r="D9" s="18" t="s">
+      <c r="D9" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="19"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="38" t="s">
+      <c r="E9" s="41"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="29" t="s">
+        <v>53</v>
+      </c>
+      <c r="H9" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="I9" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="J9" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="H9" s="34" t="s">
+      <c r="K9" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="I9" s="35" t="s">
-        <v>58</v>
-      </c>
-      <c r="J9" s="34" t="s">
-        <v>59</v>
-      </c>
-      <c r="K9" s="36" t="s">
-        <v>60</v>
-      </c>
-      <c r="L9" s="27"/>
-      <c r="M9" s="39"/>
-      <c r="N9" s="28"/>
+      <c r="L9" s="18"/>
+      <c r="M9" s="30"/>
+      <c r="N9" s="19"/>
     </row>
     <row r="10" spans="4:14">
-      <c r="D10" s="21"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="23"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="45"/>
       <c r="G10" s="12"/>
       <c r="H10" s="12"/>
       <c r="I10" s="12"/>
@@ -5118,9 +6278,9 @@
       <c r="N10" s="13"/>
     </row>
     <row r="11" spans="4:14">
-      <c r="D11" s="21"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="23"/>
+      <c r="D11" s="43"/>
+      <c r="E11" s="44"/>
+      <c r="F11" s="45"/>
       <c r="G11" s="12"/>
       <c r="H11" s="12"/>
       <c r="I11" s="12"/>
@@ -5131,35 +6291,35 @@
       <c r="N11" s="13"/>
     </row>
     <row r="12" spans="4:14" ht="14.5" thickBot="1">
-      <c r="D12" s="24"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="26"/>
+      <c r="D12" s="46"/>
+      <c r="E12" s="47"/>
+      <c r="F12" s="48"/>
       <c r="G12" s="12"/>
       <c r="H12" s="12"/>
       <c r="I12" s="12"/>
       <c r="J12" s="12"/>
       <c r="K12" s="12"/>
-      <c r="L12" s="40" t="s">
-        <v>26</v>
-      </c>
-      <c r="M12" s="40" t="s">
-        <v>48</v>
+      <c r="L12" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="M12" s="31" t="s">
+        <v>45</v>
       </c>
       <c r="N12" s="13"/>
     </row>
     <row r="13" spans="4:14">
-      <c r="D13" s="42" t="s">
-        <v>37</v>
-      </c>
-      <c r="E13" s="43"/>
-      <c r="F13" s="44"/>
+      <c r="D13" s="49" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="50"/>
+      <c r="F13" s="51"/>
       <c r="G13" s="12"/>
       <c r="H13" s="12"/>
       <c r="I13" s="12"/>
       <c r="J13" s="12"/>
       <c r="K13" s="12"/>
       <c r="L13" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="M13" s="4">
         <v>8280</v>
@@ -5167,16 +6327,16 @@
       <c r="N13" s="13"/>
     </row>
     <row r="14" spans="4:14">
-      <c r="D14" s="45"/>
-      <c r="E14" s="46"/>
-      <c r="F14" s="47"/>
+      <c r="D14" s="52"/>
+      <c r="E14" s="53"/>
+      <c r="F14" s="54"/>
       <c r="G14" s="12"/>
       <c r="H14" s="12"/>
       <c r="I14" s="12"/>
       <c r="J14" s="12"/>
       <c r="K14" s="12"/>
       <c r="L14" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="M14" s="4">
         <v>13620</v>
@@ -5184,16 +6344,16 @@
       <c r="N14" s="13"/>
     </row>
     <row r="15" spans="4:14">
-      <c r="D15" s="45"/>
-      <c r="E15" s="46"/>
-      <c r="F15" s="47"/>
+      <c r="D15" s="52"/>
+      <c r="E15" s="53"/>
+      <c r="F15" s="54"/>
       <c r="G15" s="12"/>
       <c r="H15" s="12"/>
       <c r="I15" s="12"/>
       <c r="J15" s="12"/>
       <c r="K15" s="12"/>
       <c r="L15" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="M15" s="4">
         <v>6700</v>
@@ -5201,16 +6361,16 @@
       <c r="N15" s="13"/>
     </row>
     <row r="16" spans="4:14" ht="14.5" thickBot="1">
-      <c r="D16" s="48"/>
-      <c r="E16" s="49"/>
-      <c r="F16" s="50"/>
+      <c r="D16" s="55"/>
+      <c r="E16" s="56"/>
+      <c r="F16" s="57"/>
       <c r="G16" s="12"/>
       <c r="H16" s="12"/>
       <c r="I16" s="12"/>
       <c r="J16" s="12"/>
       <c r="K16" s="12"/>
       <c r="L16" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="M16" s="4">
         <v>9413</v>
@@ -5226,10 +6386,10 @@
       <c r="I17" s="12"/>
       <c r="J17" s="12"/>
       <c r="K17" s="12"/>
-      <c r="L17" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="M17" s="41">
+      <c r="L17" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="M17" s="32">
         <f>SUM(M13:M16)</f>
         <v>38013</v>
       </c>
@@ -5310,7 +6470,7 @@
     <row r="2" spans="4:14" ht="14.5" thickBot="1"/>
     <row r="3" spans="4:14">
       <c r="D3" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
@@ -5320,14 +6480,14 @@
       <c r="J3" s="5"/>
       <c r="K3" s="10"/>
       <c r="L3" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="M3" s="5"/>
       <c r="N3" s="11"/>
     </row>
     <row r="4" spans="4:14">
       <c r="D4" s="6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
@@ -5337,7 +6497,7 @@
       <c r="J4" s="7"/>
       <c r="K4" s="12"/>
       <c r="L4" s="7" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="M4" s="7"/>
       <c r="N4" s="13"/>
@@ -5356,12 +6516,12 @@
       <c r="N5" s="15"/>
     </row>
     <row r="6" spans="4:14">
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="E6" s="19"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="32"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="23"/>
       <c r="H6" s="12"/>
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
@@ -5371,10 +6531,10 @@
       <c r="N6" s="11"/>
     </row>
     <row r="7" spans="4:14">
-      <c r="D7" s="21"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="33"/>
+      <c r="D7" s="43"/>
+      <c r="E7" s="44"/>
+      <c r="F7" s="45"/>
+      <c r="G7" s="24"/>
       <c r="H7" s="12"/>
       <c r="I7" s="12"/>
       <c r="J7" s="12"/>
@@ -5384,10 +6544,10 @@
       <c r="N7" s="13"/>
     </row>
     <row r="8" spans="4:14" ht="14.5" thickBot="1">
-      <c r="D8" s="24"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="33"/>
+      <c r="D8" s="46"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="48"/>
+      <c r="G8" s="24"/>
       <c r="H8" s="12"/>
       <c r="I8" s="12"/>
       <c r="J8" s="12"/>
@@ -5398,137 +6558,137 @@
     </row>
     <row r="9" spans="4:14">
       <c r="D9" s="58" t="s">
-        <v>68</v>
-      </c>
-      <c r="E9" s="43"/>
-      <c r="F9" s="44"/>
-      <c r="G9" s="52"/>
-      <c r="H9" s="27"/>
-      <c r="I9" s="27"/>
-      <c r="J9" s="27"/>
-      <c r="K9" s="27"/>
-      <c r="L9" s="27"/>
-      <c r="M9" s="39"/>
-      <c r="N9" s="28"/>
+        <v>65</v>
+      </c>
+      <c r="E9" s="50"/>
+      <c r="F9" s="51"/>
+      <c r="G9" s="34"/>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="18"/>
+      <c r="M9" s="30"/>
+      <c r="N9" s="19"/>
     </row>
     <row r="10" spans="4:14">
-      <c r="D10" s="45"/>
-      <c r="E10" s="46"/>
-      <c r="F10" s="47"/>
+      <c r="D10" s="52"/>
+      <c r="E10" s="53"/>
+      <c r="F10" s="54"/>
       <c r="G10" s="12"/>
       <c r="H10" s="12"/>
       <c r="I10" s="12"/>
       <c r="J10" s="12"/>
       <c r="K10" s="12"/>
       <c r="L10" s="12"/>
-      <c r="M10" s="54" t="s">
-        <v>67</v>
-      </c>
-      <c r="N10" s="56" t="s">
-        <v>65</v>
+      <c r="M10" s="36" t="s">
+        <v>64</v>
+      </c>
+      <c r="N10" s="38" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="4:14">
-      <c r="D11" s="45"/>
-      <c r="E11" s="46"/>
-      <c r="F11" s="47"/>
+      <c r="D11" s="52"/>
+      <c r="E11" s="53"/>
+      <c r="F11" s="54"/>
       <c r="G11" s="12"/>
       <c r="H11" s="12"/>
       <c r="I11" s="12"/>
       <c r="J11" s="12"/>
       <c r="K11" s="12"/>
       <c r="L11" s="12"/>
-      <c r="M11" s="33" t="s">
-        <v>61</v>
-      </c>
-      <c r="N11" s="53">
+      <c r="M11" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="N11" s="35">
         <v>5000</v>
       </c>
     </row>
     <row r="12" spans="4:14" ht="14.5" thickBot="1">
-      <c r="D12" s="48"/>
-      <c r="E12" s="49"/>
-      <c r="F12" s="50"/>
+      <c r="D12" s="55"/>
+      <c r="E12" s="56"/>
+      <c r="F12" s="57"/>
       <c r="G12" s="12"/>
       <c r="H12" s="12"/>
       <c r="I12" s="12"/>
       <c r="J12" s="12"/>
       <c r="K12" s="12"/>
       <c r="L12" s="12"/>
-      <c r="M12" s="33" t="s">
-        <v>63</v>
-      </c>
-      <c r="N12" s="53">
+      <c r="M12" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="N12" s="35">
         <v>1600</v>
       </c>
     </row>
     <row r="13" spans="4:14">
-      <c r="D13" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="E13" s="19"/>
-      <c r="F13" s="20"/>
+      <c r="D13" s="40" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="41"/>
+      <c r="F13" s="42"/>
       <c r="G13" s="12"/>
       <c r="H13" s="12"/>
       <c r="I13" s="12"/>
       <c r="J13" s="12"/>
       <c r="K13" s="12"/>
       <c r="L13" s="12"/>
-      <c r="M13" s="33" t="s">
-        <v>64</v>
-      </c>
-      <c r="N13" s="53">
+      <c r="M13" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="N13" s="35">
         <v>980</v>
       </c>
     </row>
     <row r="14" spans="4:14">
-      <c r="D14" s="21"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="23"/>
+      <c r="D14" s="43"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="45"/>
       <c r="G14" s="12"/>
       <c r="H14" s="12"/>
       <c r="I14" s="12"/>
       <c r="J14" s="12"/>
       <c r="K14" s="12"/>
       <c r="L14" s="12"/>
-      <c r="M14" s="33" t="s">
-        <v>66</v>
-      </c>
-      <c r="N14" s="53">
+      <c r="M14" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="N14" s="35">
         <v>777</v>
       </c>
     </row>
     <row r="15" spans="4:14">
-      <c r="D15" s="21"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="23"/>
+      <c r="D15" s="43"/>
+      <c r="E15" s="44"/>
+      <c r="F15" s="45"/>
       <c r="G15" s="12"/>
       <c r="H15" s="12"/>
       <c r="I15" s="12"/>
       <c r="J15" s="12"/>
       <c r="K15" s="12"/>
       <c r="L15" s="12"/>
-      <c r="M15" s="33" t="s">
-        <v>62</v>
-      </c>
-      <c r="N15" s="53">
+      <c r="M15" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="N15" s="35">
         <v>1987</v>
       </c>
     </row>
     <row r="16" spans="4:14" ht="14.5" thickBot="1">
-      <c r="D16" s="24"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="26"/>
+      <c r="D16" s="46"/>
+      <c r="E16" s="47"/>
+      <c r="F16" s="48"/>
       <c r="G16" s="12"/>
       <c r="H16" s="12"/>
       <c r="I16" s="12"/>
       <c r="J16" s="12"/>
       <c r="K16" s="12"/>
       <c r="L16" s="12"/>
-      <c r="M16" s="55" t="s">
-        <v>42</v>
-      </c>
-      <c r="N16" s="57">
+      <c r="M16" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="N16" s="39">
         <f>SUM(N11:N15)</f>
         <v>10344</v>
       </c>
@@ -5595,4 +6755,2165 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BF177E8-58E9-49D2-A1D2-A791BCE695DC}">
+  <dimension ref="D2:O51"/>
+  <sheetViews>
+    <sheetView topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23:O51"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14"/>
+  <cols>
+    <col min="1" max="6" width="8.6640625" style="4"/>
+    <col min="7" max="7" width="12.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.08203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.58203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="18.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.25" style="4" customWidth="1"/>
+    <col min="13" max="13" width="8.6640625" style="4"/>
+    <col min="14" max="14" width="18.9140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="4" style="4" customWidth="1"/>
+    <col min="16" max="16384" width="8.6640625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="4:15" ht="14.5" thickBot="1"/>
+    <row r="3" spans="4:15">
+      <c r="D3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="11"/>
+    </row>
+    <row r="4" spans="4:15">
+      <c r="D4" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="13"/>
+    </row>
+    <row r="5" spans="4:15" ht="14.5" thickBot="1">
+      <c r="D5" s="8"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="14"/>
+      <c r="O5" s="15"/>
+    </row>
+    <row r="6" spans="4:15">
+      <c r="D6" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="41"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="10"/>
+      <c r="O6" s="11"/>
+    </row>
+    <row r="7" spans="4:15">
+      <c r="D7" s="43"/>
+      <c r="E7" s="44"/>
+      <c r="F7" s="45"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="12"/>
+      <c r="N7" s="12"/>
+      <c r="O7" s="13"/>
+    </row>
+    <row r="8" spans="4:15" ht="14.5" thickBot="1">
+      <c r="D8" s="46"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="48"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="12"/>
+      <c r="N8" s="12"/>
+      <c r="O8" s="13"/>
+    </row>
+    <row r="9" spans="4:15">
+      <c r="D9" s="60" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="61"/>
+      <c r="F9" s="62"/>
+      <c r="G9" s="24"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="12"/>
+      <c r="N9" s="12"/>
+      <c r="O9" s="13"/>
+    </row>
+    <row r="10" spans="4:15">
+      <c r="D10" s="63"/>
+      <c r="E10" s="64"/>
+      <c r="F10" s="65"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="71" t="s">
+        <v>68</v>
+      </c>
+      <c r="I10" s="71" t="s">
+        <v>69</v>
+      </c>
+      <c r="J10" s="71" t="s">
+        <v>83</v>
+      </c>
+      <c r="K10" s="12"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="12"/>
+      <c r="N10" s="12"/>
+      <c r="O10" s="13"/>
+    </row>
+    <row r="11" spans="4:15">
+      <c r="D11" s="63"/>
+      <c r="E11" s="64"/>
+      <c r="F11" s="65"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="I11" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="J11" s="70">
+        <v>16300508.050000001</v>
+      </c>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="12"/>
+      <c r="O11" s="13"/>
+    </row>
+    <row r="12" spans="4:15" ht="14.5" thickBot="1">
+      <c r="D12" s="66"/>
+      <c r="E12" s="67"/>
+      <c r="F12" s="68"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="I12" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="J12" s="70">
+        <v>9789644.9800000004</v>
+      </c>
+      <c r="K12" s="12"/>
+      <c r="L12" s="31"/>
+      <c r="M12" s="31"/>
+      <c r="N12" s="31"/>
+      <c r="O12" s="13"/>
+    </row>
+    <row r="13" spans="4:15">
+      <c r="D13" s="40" t="s">
+        <v>67</v>
+      </c>
+      <c r="E13" s="41"/>
+      <c r="F13" s="42"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="I13" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="J13" s="70">
+        <v>6788688.0499999998</v>
+      </c>
+      <c r="K13" s="12"/>
+      <c r="O13" s="13"/>
+    </row>
+    <row r="14" spans="4:15">
+      <c r="D14" s="43"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="45"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="I14" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="J14" s="70">
+        <v>6689002</v>
+      </c>
+      <c r="K14" s="12"/>
+      <c r="O14" s="13"/>
+    </row>
+    <row r="15" spans="4:15">
+      <c r="D15" s="43"/>
+      <c r="E15" s="44"/>
+      <c r="F15" s="45"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="I15" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="J15" s="70">
+        <v>5776559.9800000004</v>
+      </c>
+      <c r="K15" s="12"/>
+      <c r="O15" s="13"/>
+    </row>
+    <row r="16" spans="4:15" ht="14.5" thickBot="1">
+      <c r="D16" s="46"/>
+      <c r="E16" s="47"/>
+      <c r="F16" s="48"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="I16" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="J16" s="70">
+        <v>3002993.99</v>
+      </c>
+      <c r="K16" s="12"/>
+      <c r="O16" s="13"/>
+    </row>
+    <row r="17" spans="4:15" ht="14.5" thickBot="1">
+      <c r="D17" s="16"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="72" t="s">
+        <v>39</v>
+      </c>
+      <c r="I17" s="72"/>
+      <c r="J17" s="73">
+        <f>SUM(J11:J16)</f>
+        <v>48347397.050000004</v>
+      </c>
+      <c r="K17" s="12"/>
+      <c r="O17" s="13"/>
+    </row>
+    <row r="18" spans="4:15">
+      <c r="D18" s="16"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="12"/>
+      <c r="M18" s="12"/>
+      <c r="N18" s="12"/>
+      <c r="O18" s="13"/>
+    </row>
+    <row r="19" spans="4:15">
+      <c r="D19" s="16"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="12"/>
+      <c r="M19" s="12"/>
+      <c r="N19" s="12"/>
+      <c r="O19" s="13"/>
+    </row>
+    <row r="20" spans="4:15" ht="14.5" thickBot="1">
+      <c r="D20" s="17"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="14"/>
+      <c r="L20" s="14"/>
+      <c r="M20" s="14"/>
+      <c r="N20" s="14"/>
+      <c r="O20" s="15"/>
+    </row>
+    <row r="22" spans="4:15" ht="14.5" thickBot="1"/>
+    <row r="23" spans="4:15">
+      <c r="D23" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="M23" s="5"/>
+      <c r="N23" s="5"/>
+      <c r="O23" s="11"/>
+    </row>
+    <row r="24" spans="4:15">
+      <c r="D24" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="7"/>
+      <c r="K24" s="12"/>
+      <c r="L24" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="M24" s="7"/>
+      <c r="N24" s="7"/>
+      <c r="O24" s="13"/>
+    </row>
+    <row r="25" spans="4:15" ht="14.5" thickBot="1">
+      <c r="D25" s="8"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="9"/>
+      <c r="K25" s="9"/>
+      <c r="L25" s="9"/>
+      <c r="M25" s="14"/>
+      <c r="N25" s="14"/>
+      <c r="O25" s="15"/>
+    </row>
+    <row r="26" spans="4:15">
+      <c r="D26" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26" s="41"/>
+      <c r="F26" s="42"/>
+      <c r="G26" s="23"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="10"/>
+      <c r="J26" s="10"/>
+      <c r="K26" s="10"/>
+      <c r="L26" s="10"/>
+      <c r="M26" s="10"/>
+      <c r="N26" s="10"/>
+      <c r="O26" s="11"/>
+    </row>
+    <row r="27" spans="4:15">
+      <c r="D27" s="43"/>
+      <c r="E27" s="44"/>
+      <c r="F27" s="45"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="79" t="s">
+        <v>68</v>
+      </c>
+      <c r="I27" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="J27" s="12"/>
+      <c r="M27" s="12"/>
+      <c r="N27" s="12"/>
+      <c r="O27" s="13"/>
+    </row>
+    <row r="28" spans="4:15" ht="14.5" thickBot="1">
+      <c r="D28" s="46"/>
+      <c r="E28" s="47"/>
+      <c r="F28" s="48"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="79" t="s">
+        <v>101</v>
+      </c>
+      <c r="I28" s="78" t="s">
+        <v>84</v>
+      </c>
+      <c r="J28" s="12"/>
+      <c r="M28" s="12"/>
+      <c r="N28" s="12"/>
+      <c r="O28" s="13"/>
+    </row>
+    <row r="29" spans="4:15">
+      <c r="D29" s="60" t="s">
+        <v>13</v>
+      </c>
+      <c r="E29" s="61"/>
+      <c r="F29" s="62"/>
+      <c r="G29" s="24"/>
+      <c r="H29" s="79" t="s">
+        <v>69</v>
+      </c>
+      <c r="I29" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="J29" s="12"/>
+      <c r="K29" s="12"/>
+      <c r="L29" s="12"/>
+      <c r="M29" s="12"/>
+      <c r="N29" s="12"/>
+      <c r="O29" s="13"/>
+    </row>
+    <row r="30" spans="4:15">
+      <c r="D30" s="63"/>
+      <c r="E30" s="64"/>
+      <c r="F30" s="65"/>
+      <c r="G30" s="24"/>
+      <c r="H30" s="12"/>
+      <c r="I30" s="12"/>
+      <c r="J30" s="12"/>
+      <c r="K30" s="12"/>
+      <c r="L30" s="12"/>
+      <c r="M30" s="12"/>
+      <c r="N30" s="12"/>
+      <c r="O30" s="13"/>
+    </row>
+    <row r="31" spans="4:15">
+      <c r="D31" s="63"/>
+      <c r="E31" s="64"/>
+      <c r="F31" s="65"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="71" t="s">
+        <v>40</v>
+      </c>
+      <c r="I31" s="12"/>
+      <c r="J31" s="12"/>
+      <c r="K31" s="12"/>
+      <c r="L31" s="12"/>
+      <c r="M31" s="12"/>
+      <c r="N31" s="12"/>
+      <c r="O31" s="13"/>
+    </row>
+    <row r="32" spans="4:15">
+      <c r="D32" s="63"/>
+      <c r="E32" s="64"/>
+      <c r="F32" s="65"/>
+      <c r="G32" s="12"/>
+      <c r="H32" s="74" t="s">
+        <v>92</v>
+      </c>
+      <c r="I32" s="74" t="s">
+        <v>89</v>
+      </c>
+      <c r="J32" s="74" t="s">
+        <v>85</v>
+      </c>
+      <c r="K32" s="74" t="s">
+        <v>86</v>
+      </c>
+      <c r="L32" s="74" t="s">
+        <v>87</v>
+      </c>
+      <c r="M32" s="74" t="s">
+        <v>90</v>
+      </c>
+      <c r="N32" s="74" t="s">
+        <v>100</v>
+      </c>
+      <c r="O32" s="13"/>
+    </row>
+    <row r="33" spans="4:15" ht="14.5" thickBot="1">
+      <c r="D33" s="66"/>
+      <c r="E33" s="67"/>
+      <c r="F33" s="68"/>
+      <c r="G33" s="12"/>
+      <c r="H33" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="I33" s="12">
+        <v>80000</v>
+      </c>
+      <c r="J33" s="12">
+        <f>I33*K33</f>
+        <v>5084000</v>
+      </c>
+      <c r="K33" s="12">
+        <v>63.55</v>
+      </c>
+      <c r="L33" s="12">
+        <v>60.05</v>
+      </c>
+      <c r="M33" s="24">
+        <f>I33*K33 - I33*L33</f>
+        <v>280000</v>
+      </c>
+      <c r="N33" s="24">
+        <v>6000</v>
+      </c>
+      <c r="O33" s="13"/>
+    </row>
+    <row r="34" spans="4:15">
+      <c r="D34" s="40" t="s">
+        <v>67</v>
+      </c>
+      <c r="E34" s="41"/>
+      <c r="F34" s="42"/>
+      <c r="G34" s="12"/>
+      <c r="H34" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="I34" s="12">
+        <v>10000</v>
+      </c>
+      <c r="J34" s="12">
+        <f>I34*K34</f>
+        <v>2706000</v>
+      </c>
+      <c r="K34" s="12">
+        <v>270.60000000000002</v>
+      </c>
+      <c r="L34" s="12">
+        <v>180.5</v>
+      </c>
+      <c r="M34" s="24">
+        <f>I34*K34 - I34*L34</f>
+        <v>901000</v>
+      </c>
+      <c r="N34" s="24">
+        <v>3000</v>
+      </c>
+      <c r="O34" s="13"/>
+    </row>
+    <row r="35" spans="4:15" ht="14.5" thickBot="1">
+      <c r="D35" s="43"/>
+      <c r="E35" s="44"/>
+      <c r="F35" s="45"/>
+      <c r="G35" s="12"/>
+      <c r="H35" s="75" t="s">
+        <v>39</v>
+      </c>
+      <c r="I35" s="75"/>
+      <c r="J35" s="75">
+        <f>SUM(J33:J34)</f>
+        <v>7790000</v>
+      </c>
+      <c r="K35" s="75"/>
+      <c r="L35" s="75"/>
+      <c r="M35" s="76">
+        <f>SUM(M33:M34)</f>
+        <v>1181000</v>
+      </c>
+      <c r="N35" s="76">
+        <f>SUM(N33:N34)</f>
+        <v>9000</v>
+      </c>
+      <c r="O35" s="13"/>
+    </row>
+    <row r="36" spans="4:15">
+      <c r="D36" s="43"/>
+      <c r="E36" s="44"/>
+      <c r="F36" s="45"/>
+      <c r="G36" s="12"/>
+      <c r="H36" s="12"/>
+      <c r="I36" s="12"/>
+      <c r="J36" s="12"/>
+      <c r="K36" s="12"/>
+      <c r="L36" s="12"/>
+      <c r="M36" s="12"/>
+      <c r="N36" s="12"/>
+      <c r="O36" s="13"/>
+    </row>
+    <row r="37" spans="4:15" ht="14.5" thickBot="1">
+      <c r="D37" s="46"/>
+      <c r="E37" s="47"/>
+      <c r="F37" s="48"/>
+      <c r="G37" s="12"/>
+      <c r="H37" s="71" t="s">
+        <v>41</v>
+      </c>
+      <c r="I37" s="78"/>
+      <c r="J37" s="12"/>
+      <c r="K37" s="70"/>
+      <c r="L37" s="12"/>
+      <c r="M37" s="12"/>
+      <c r="N37" s="12"/>
+      <c r="O37" s="13"/>
+    </row>
+    <row r="38" spans="4:15">
+      <c r="D38" s="16"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="13"/>
+      <c r="G38" s="12"/>
+      <c r="H38" s="74" t="s">
+        <v>92</v>
+      </c>
+      <c r="I38" s="74" t="s">
+        <v>89</v>
+      </c>
+      <c r="J38" s="74" t="s">
+        <v>85</v>
+      </c>
+      <c r="K38" s="74" t="s">
+        <v>86</v>
+      </c>
+      <c r="L38" s="74" t="s">
+        <v>87</v>
+      </c>
+      <c r="M38" s="74" t="s">
+        <v>90</v>
+      </c>
+      <c r="N38" s="74" t="s">
+        <v>100</v>
+      </c>
+      <c r="O38" s="13"/>
+    </row>
+    <row r="39" spans="4:15">
+      <c r="D39" s="16"/>
+      <c r="E39" s="12"/>
+      <c r="F39" s="13"/>
+      <c r="G39" s="12"/>
+      <c r="H39" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="I39" s="12">
+        <v>1000000</v>
+      </c>
+      <c r="J39" s="12">
+        <f>I39*K39</f>
+        <v>2340000</v>
+      </c>
+      <c r="K39" s="12">
+        <v>2.34</v>
+      </c>
+      <c r="L39" s="12">
+        <v>1.05</v>
+      </c>
+      <c r="M39" s="12">
+        <f>I39*K39 - I39*L39</f>
+        <v>1290000</v>
+      </c>
+      <c r="N39" s="12">
+        <v>-3000</v>
+      </c>
+      <c r="O39" s="13"/>
+    </row>
+    <row r="40" spans="4:15" ht="14.5" thickBot="1">
+      <c r="D40" s="16"/>
+      <c r="E40" s="12"/>
+      <c r="F40" s="13"/>
+      <c r="G40" s="12"/>
+      <c r="H40" s="75" t="s">
+        <v>39</v>
+      </c>
+      <c r="I40" s="75"/>
+      <c r="J40" s="75">
+        <f>SUM(J38:J39)</f>
+        <v>2340000</v>
+      </c>
+      <c r="K40" s="75"/>
+      <c r="L40" s="75"/>
+      <c r="M40" s="76">
+        <f>SUM(M38:M39)</f>
+        <v>1290000</v>
+      </c>
+      <c r="N40" s="76">
+        <f>SUM(N38:N39)</f>
+        <v>-3000</v>
+      </c>
+      <c r="O40" s="13"/>
+    </row>
+    <row r="41" spans="4:15">
+      <c r="D41" s="16"/>
+      <c r="E41" s="12"/>
+      <c r="F41" s="13"/>
+      <c r="G41" s="12"/>
+      <c r="H41" s="12"/>
+      <c r="I41" s="12"/>
+      <c r="J41" s="12"/>
+      <c r="K41" s="12"/>
+      <c r="L41" s="12"/>
+      <c r="M41" s="12"/>
+      <c r="N41" s="12"/>
+      <c r="O41" s="13"/>
+    </row>
+    <row r="42" spans="4:15">
+      <c r="D42" s="16"/>
+      <c r="E42" s="12"/>
+      <c r="F42" s="13"/>
+      <c r="G42" s="12"/>
+      <c r="H42" s="71" t="s">
+        <v>44</v>
+      </c>
+      <c r="I42" s="78"/>
+      <c r="J42" s="12"/>
+      <c r="K42" s="70"/>
+      <c r="L42" s="12"/>
+      <c r="M42" s="12"/>
+      <c r="N42" s="12"/>
+      <c r="O42" s="13"/>
+    </row>
+    <row r="43" spans="4:15">
+      <c r="D43" s="16"/>
+      <c r="E43" s="12"/>
+      <c r="F43" s="13"/>
+      <c r="G43" s="12"/>
+      <c r="H43" s="74" t="s">
+        <v>94</v>
+      </c>
+      <c r="I43" s="74" t="s">
+        <v>96</v>
+      </c>
+      <c r="J43" s="74" t="s">
+        <v>97</v>
+      </c>
+      <c r="K43" s="74" t="s">
+        <v>98</v>
+      </c>
+      <c r="L43" s="74" t="s">
+        <v>99</v>
+      </c>
+      <c r="M43" s="74" t="s">
+        <v>90</v>
+      </c>
+      <c r="N43" s="74" t="s">
+        <v>100</v>
+      </c>
+      <c r="O43" s="13"/>
+    </row>
+    <row r="44" spans="4:15">
+      <c r="D44" s="16"/>
+      <c r="E44" s="12"/>
+      <c r="F44" s="13"/>
+      <c r="G44" s="12"/>
+      <c r="H44" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="I44" s="12">
+        <v>500000</v>
+      </c>
+      <c r="J44" s="12">
+        <f>I44/K44</f>
+        <v>63928.808878432974</v>
+      </c>
+      <c r="K44" s="12">
+        <v>7.8212000000000002</v>
+      </c>
+      <c r="L44" s="12">
+        <v>7.8010000000000002</v>
+      </c>
+      <c r="M44" s="12">
+        <f>I44 / K44 - I44 /L44</f>
+        <v>-165.53800017233152</v>
+      </c>
+      <c r="N44" s="12">
+        <f>M44</f>
+        <v>-165.53800017233152</v>
+      </c>
+      <c r="O44" s="13"/>
+    </row>
+    <row r="45" spans="4:15" ht="14.5" thickBot="1">
+      <c r="D45" s="16"/>
+      <c r="E45" s="12"/>
+      <c r="F45" s="13"/>
+      <c r="G45" s="12"/>
+      <c r="H45" s="75" t="s">
+        <v>39</v>
+      </c>
+      <c r="I45" s="75"/>
+      <c r="J45" s="75">
+        <f>SUM(J43:J44)</f>
+        <v>63928.808878432974</v>
+      </c>
+      <c r="K45" s="75"/>
+      <c r="L45" s="75"/>
+      <c r="M45" s="76">
+        <f>SUM(M43:M44)</f>
+        <v>-165.53800017233152</v>
+      </c>
+      <c r="N45" s="76">
+        <f>SUM(N43:N44)</f>
+        <v>-165.53800017233152</v>
+      </c>
+      <c r="O45" s="13"/>
+    </row>
+    <row r="46" spans="4:15">
+      <c r="D46" s="16"/>
+      <c r="E46" s="12"/>
+      <c r="F46" s="13"/>
+      <c r="G46" s="12"/>
+      <c r="H46" s="12"/>
+      <c r="I46" s="12"/>
+      <c r="J46" s="12"/>
+      <c r="K46" s="12"/>
+      <c r="L46" s="12"/>
+      <c r="M46" s="24"/>
+      <c r="N46" s="24"/>
+      <c r="O46" s="13"/>
+    </row>
+    <row r="47" spans="4:15">
+      <c r="D47" s="16"/>
+      <c r="E47" s="12"/>
+      <c r="F47" s="13"/>
+      <c r="G47" s="12"/>
+      <c r="H47" s="71" t="s">
+        <v>102</v>
+      </c>
+      <c r="I47" s="12"/>
+      <c r="J47" s="12"/>
+      <c r="K47" s="12"/>
+      <c r="L47" s="12"/>
+      <c r="M47" s="24"/>
+      <c r="N47" s="24"/>
+      <c r="O47" s="13"/>
+    </row>
+    <row r="48" spans="4:15">
+      <c r="D48" s="16"/>
+      <c r="E48" s="12"/>
+      <c r="F48" s="13"/>
+      <c r="G48" s="12"/>
+      <c r="H48" s="81" t="s">
+        <v>40</v>
+      </c>
+      <c r="I48" s="81" t="s">
+        <v>41</v>
+      </c>
+      <c r="J48" s="81" t="s">
+        <v>44</v>
+      </c>
+      <c r="K48" s="81" t="s">
+        <v>42</v>
+      </c>
+      <c r="L48" s="81" t="s">
+        <v>103</v>
+      </c>
+      <c r="M48" s="81" t="s">
+        <v>70</v>
+      </c>
+      <c r="N48" s="81" t="s">
+        <v>104</v>
+      </c>
+      <c r="O48" s="13"/>
+    </row>
+    <row r="49" spans="4:15">
+      <c r="D49" s="16"/>
+      <c r="E49" s="12"/>
+      <c r="F49" s="13"/>
+      <c r="G49" s="12"/>
+      <c r="H49" s="82">
+        <v>7790000</v>
+      </c>
+      <c r="I49" s="82">
+        <v>2340000</v>
+      </c>
+      <c r="J49" s="82">
+        <v>50000</v>
+      </c>
+      <c r="K49" s="82">
+        <v>0</v>
+      </c>
+      <c r="L49" s="82">
+        <f>SUM(H49:K49)</f>
+        <v>10180000</v>
+      </c>
+      <c r="M49" s="83">
+        <f>SUM(M35+M40+M45)</f>
+        <v>2470834.4619998275</v>
+      </c>
+      <c r="N49" s="83">
+        <f>SUM(N35+N40+N45)</f>
+        <v>5834.4619998276685</v>
+      </c>
+      <c r="O49" s="13"/>
+    </row>
+    <row r="50" spans="4:15">
+      <c r="D50" s="16"/>
+      <c r="E50" s="12"/>
+      <c r="F50" s="13"/>
+      <c r="G50" s="12"/>
+      <c r="H50" s="12"/>
+      <c r="I50" s="12"/>
+      <c r="J50" s="12"/>
+      <c r="K50" s="12"/>
+      <c r="L50" s="12"/>
+      <c r="M50" s="24"/>
+      <c r="N50" s="24"/>
+      <c r="O50" s="13"/>
+    </row>
+    <row r="51" spans="4:15" ht="14.5" thickBot="1">
+      <c r="D51" s="17"/>
+      <c r="E51" s="14"/>
+      <c r="F51" s="15"/>
+      <c r="G51" s="14"/>
+      <c r="H51" s="14"/>
+      <c r="I51" s="14"/>
+      <c r="J51" s="14"/>
+      <c r="K51" s="14"/>
+      <c r="L51" s="14"/>
+      <c r="M51" s="14"/>
+      <c r="N51" s="14"/>
+      <c r="O51" s="15"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="D6:F8"/>
+    <mergeCell ref="D9:F12"/>
+    <mergeCell ref="D13:F16"/>
+    <mergeCell ref="D26:F28"/>
+    <mergeCell ref="D29:F33"/>
+    <mergeCell ref="D34:F37"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAEFB75A-56EA-40E4-9B3E-55B39FAB2241}">
+  <dimension ref="D5:Q32"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="T13" sqref="T13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14"/>
+  <cols>
+    <col min="1" max="7" width="8.6640625" style="84"/>
+    <col min="8" max="8" width="11.75" style="84" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="9.33203125" style="84" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.83203125" style="84" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.6640625" style="84"/>
+    <col min="13" max="13" width="4.4140625" style="84" customWidth="1"/>
+    <col min="14" max="14" width="6.58203125" style="84" customWidth="1"/>
+    <col min="15" max="16384" width="8.6640625" style="84"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="4:17" ht="14.5" thickBot="1"/>
+    <row r="6" spans="4:17">
+      <c r="D6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="11"/>
+    </row>
+    <row r="7" spans="4:17">
+      <c r="D7" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="12"/>
+      <c r="N7" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="O7" s="7"/>
+      <c r="P7" s="7"/>
+      <c r="Q7" s="13"/>
+    </row>
+    <row r="8" spans="4:17" ht="14.5" thickBot="1">
+      <c r="D8" s="8"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="14"/>
+      <c r="P8" s="14"/>
+      <c r="Q8" s="15"/>
+    </row>
+    <row r="9" spans="4:17">
+      <c r="D9" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="41"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="10"/>
+      <c r="O9" s="10"/>
+      <c r="P9" s="10"/>
+      <c r="Q9" s="11"/>
+    </row>
+    <row r="10" spans="4:17" ht="14.5" thickBot="1">
+      <c r="D10" s="43"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="45"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="24"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="12"/>
+      <c r="N10" s="12"/>
+      <c r="O10" s="12"/>
+      <c r="P10" s="12"/>
+      <c r="Q10" s="13"/>
+    </row>
+    <row r="11" spans="4:17" ht="14.5" thickBot="1">
+      <c r="D11" s="46"/>
+      <c r="E11" s="47"/>
+      <c r="F11" s="48"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="103" t="s">
+        <v>107</v>
+      </c>
+      <c r="I11" s="104" t="s">
+        <v>108</v>
+      </c>
+      <c r="J11" s="101"/>
+      <c r="K11" s="105" t="s">
+        <v>113</v>
+      </c>
+      <c r="L11" s="106" t="s">
+        <v>114</v>
+      </c>
+      <c r="M11" s="12"/>
+      <c r="N11" s="12"/>
+      <c r="O11" s="12"/>
+      <c r="P11" s="12"/>
+      <c r="Q11" s="13"/>
+    </row>
+    <row r="12" spans="4:17" ht="14.5" thickBot="1">
+      <c r="D12" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="41"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="118"/>
+      <c r="I12" s="101"/>
+      <c r="J12" s="101"/>
+      <c r="K12" s="100"/>
+      <c r="L12" s="102"/>
+      <c r="M12" s="12"/>
+      <c r="N12" s="12"/>
+      <c r="O12" s="12"/>
+      <c r="P12" s="12"/>
+      <c r="Q12" s="13"/>
+    </row>
+    <row r="13" spans="4:17">
+      <c r="D13" s="43"/>
+      <c r="E13" s="44"/>
+      <c r="F13" s="45"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="117" t="s">
+        <v>134</v>
+      </c>
+      <c r="I13" s="125" t="s">
+        <v>137</v>
+      </c>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="13"/>
+      <c r="M13" s="12"/>
+      <c r="N13" s="96" t="s">
+        <v>116</v>
+      </c>
+      <c r="O13" s="87"/>
+      <c r="P13" s="130" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q13" s="13"/>
+    </row>
+    <row r="14" spans="4:17">
+      <c r="D14" s="43"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="45"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="116" t="s">
+        <v>109</v>
+      </c>
+      <c r="I14" s="126" t="s">
+        <v>121</v>
+      </c>
+      <c r="J14" s="69"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="13"/>
+      <c r="M14" s="12"/>
+      <c r="N14" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="O14" s="97"/>
+      <c r="P14" s="131" t="s">
+        <v>141</v>
+      </c>
+      <c r="Q14" s="13"/>
+    </row>
+    <row r="15" spans="4:17">
+      <c r="D15" s="43"/>
+      <c r="E15" s="44"/>
+      <c r="F15" s="45"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="116" t="s">
+        <v>110</v>
+      </c>
+      <c r="I15" s="126">
+        <v>6000</v>
+      </c>
+      <c r="J15" s="86"/>
+      <c r="K15" s="86"/>
+      <c r="L15" s="90"/>
+      <c r="M15" s="86"/>
+      <c r="N15" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="O15" s="86"/>
+      <c r="P15" s="132" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q15" s="13"/>
+    </row>
+    <row r="16" spans="4:17" ht="14.5" thickBot="1">
+      <c r="D16" s="46"/>
+      <c r="E16" s="47"/>
+      <c r="F16" s="48"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="116" t="s">
+        <v>115</v>
+      </c>
+      <c r="I16" s="127" t="s">
+        <v>49</v>
+      </c>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="13"/>
+      <c r="M16" s="12"/>
+      <c r="N16" s="16"/>
+      <c r="O16" s="24"/>
+      <c r="P16" s="35"/>
+      <c r="Q16" s="13"/>
+    </row>
+    <row r="17" spans="4:17">
+      <c r="D17" s="85" t="s">
+        <v>105</v>
+      </c>
+      <c r="E17" s="61"/>
+      <c r="F17" s="62"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="116" t="s">
+        <v>111</v>
+      </c>
+      <c r="I17" s="127">
+        <v>61.05</v>
+      </c>
+      <c r="J17" s="12"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="13"/>
+      <c r="M17" s="12"/>
+      <c r="N17" s="16"/>
+      <c r="O17" s="24"/>
+      <c r="P17" s="35"/>
+      <c r="Q17" s="13"/>
+    </row>
+    <row r="18" spans="4:17">
+      <c r="D18" s="63"/>
+      <c r="E18" s="64"/>
+      <c r="F18" s="65"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="116" t="s">
+        <v>112</v>
+      </c>
+      <c r="I18" s="127" t="s">
+        <v>138</v>
+      </c>
+      <c r="J18" s="12"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="13"/>
+      <c r="M18" s="12"/>
+      <c r="N18" s="16"/>
+      <c r="O18" s="24"/>
+      <c r="P18" s="35"/>
+      <c r="Q18" s="13"/>
+    </row>
+    <row r="19" spans="4:17">
+      <c r="D19" s="63"/>
+      <c r="E19" s="64"/>
+      <c r="F19" s="65"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="116" t="s">
+        <v>135</v>
+      </c>
+      <c r="I19" s="127" t="s">
+        <v>139</v>
+      </c>
+      <c r="J19" s="12"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="13"/>
+      <c r="M19" s="12"/>
+      <c r="N19" s="16"/>
+      <c r="O19" s="12"/>
+      <c r="P19" s="13"/>
+      <c r="Q19" s="13"/>
+    </row>
+    <row r="20" spans="4:17" ht="14.5" thickBot="1">
+      <c r="D20" s="66"/>
+      <c r="E20" s="67"/>
+      <c r="F20" s="68"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="88"/>
+      <c r="I20" s="69"/>
+      <c r="J20" s="69"/>
+      <c r="K20" s="78"/>
+      <c r="L20" s="13"/>
+      <c r="M20" s="70"/>
+      <c r="N20" s="16"/>
+      <c r="O20" s="12"/>
+      <c r="P20" s="13"/>
+      <c r="Q20" s="13"/>
+    </row>
+    <row r="21" spans="4:17">
+      <c r="D21" s="16"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="89"/>
+      <c r="I21" s="86"/>
+      <c r="J21" s="86"/>
+      <c r="K21" s="86"/>
+      <c r="L21" s="90"/>
+      <c r="M21" s="86"/>
+      <c r="N21" s="89"/>
+      <c r="O21" s="86"/>
+      <c r="P21" s="90"/>
+      <c r="Q21" s="13"/>
+    </row>
+    <row r="22" spans="4:17">
+      <c r="D22" s="16"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="16"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="12"/>
+      <c r="K22" s="12"/>
+      <c r="L22" s="13"/>
+      <c r="M22" s="12"/>
+      <c r="N22" s="16"/>
+      <c r="O22" s="12"/>
+      <c r="P22" s="13"/>
+      <c r="Q22" s="13"/>
+    </row>
+    <row r="23" spans="4:17" ht="14.5" thickBot="1">
+      <c r="D23" s="16"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="92"/>
+      <c r="I23" s="93"/>
+      <c r="J23" s="93"/>
+      <c r="K23" s="94"/>
+      <c r="L23" s="15"/>
+      <c r="M23" s="70"/>
+      <c r="N23" s="17"/>
+      <c r="O23" s="14"/>
+      <c r="P23" s="15"/>
+      <c r="Q23" s="13"/>
+    </row>
+    <row r="24" spans="4:17" ht="14.5" thickBot="1">
+      <c r="D24" s="16"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="86"/>
+      <c r="I24" s="86"/>
+      <c r="J24" s="86"/>
+      <c r="K24" s="86"/>
+      <c r="L24" s="86"/>
+      <c r="M24" s="86"/>
+      <c r="N24" s="86"/>
+      <c r="O24" s="86"/>
+      <c r="P24" s="86"/>
+      <c r="Q24" s="13"/>
+    </row>
+    <row r="25" spans="4:17">
+      <c r="D25" s="16"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="128" t="s">
+        <v>120</v>
+      </c>
+      <c r="I25" s="10"/>
+      <c r="J25" s="10"/>
+      <c r="K25" s="10"/>
+      <c r="L25" s="11"/>
+      <c r="M25" s="12"/>
+      <c r="N25" s="128" t="s">
+        <v>133</v>
+      </c>
+      <c r="O25" s="129"/>
+      <c r="P25" s="11"/>
+      <c r="Q25" s="13"/>
+    </row>
+    <row r="26" spans="4:17">
+      <c r="D26" s="16"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="119" t="s">
+        <v>118</v>
+      </c>
+      <c r="I26" s="120" t="s">
+        <v>119</v>
+      </c>
+      <c r="J26" s="120" t="s">
+        <v>110</v>
+      </c>
+      <c r="K26" s="120" t="s">
+        <v>103</v>
+      </c>
+      <c r="L26" s="121" t="s">
+        <v>122</v>
+      </c>
+      <c r="M26" s="12"/>
+      <c r="N26" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="O26" s="24"/>
+      <c r="P26" s="35"/>
+      <c r="Q26" s="13"/>
+    </row>
+    <row r="27" spans="4:17" ht="14.5" thickBot="1">
+      <c r="D27" s="16"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="122" t="s">
+        <v>121</v>
+      </c>
+      <c r="I27" s="123">
+        <v>60.5</v>
+      </c>
+      <c r="J27" s="123">
+        <v>80000</v>
+      </c>
+      <c r="K27" s="123">
+        <f>J27*I27</f>
+        <v>4840000</v>
+      </c>
+      <c r="L27" s="124" t="s">
+        <v>49</v>
+      </c>
+      <c r="M27" s="12"/>
+      <c r="N27" s="16"/>
+      <c r="O27" s="24"/>
+      <c r="P27" s="35"/>
+      <c r="Q27" s="13"/>
+    </row>
+    <row r="28" spans="4:17" ht="14.5" thickBot="1">
+      <c r="D28" s="16"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="88"/>
+      <c r="I28" s="69"/>
+      <c r="J28" s="69"/>
+      <c r="K28" s="12"/>
+      <c r="L28" s="13"/>
+      <c r="M28" s="12"/>
+      <c r="N28" s="17"/>
+      <c r="O28" s="77"/>
+      <c r="P28" s="111"/>
+      <c r="Q28" s="13"/>
+    </row>
+    <row r="29" spans="4:17">
+      <c r="D29" s="16"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="98"/>
+      <c r="I29" s="80"/>
+      <c r="J29" s="80"/>
+      <c r="K29" s="80"/>
+      <c r="L29" s="99"/>
+      <c r="M29" s="80"/>
+      <c r="N29" s="80"/>
+      <c r="O29" s="80"/>
+      <c r="P29" s="80"/>
+      <c r="Q29" s="13"/>
+    </row>
+    <row r="30" spans="4:17" ht="14.5" thickBot="1">
+      <c r="D30" s="16"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="17"/>
+      <c r="I30" s="14"/>
+      <c r="J30" s="14"/>
+      <c r="K30" s="14"/>
+      <c r="L30" s="15"/>
+      <c r="M30" s="12"/>
+      <c r="N30" s="12"/>
+      <c r="O30" s="24"/>
+      <c r="P30" s="24"/>
+      <c r="Q30" s="13"/>
+    </row>
+    <row r="31" spans="4:17">
+      <c r="D31" s="16"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="12"/>
+      <c r="I31" s="12"/>
+      <c r="J31" s="12"/>
+      <c r="K31" s="12"/>
+      <c r="L31" s="12"/>
+      <c r="M31" s="12"/>
+      <c r="N31" s="12"/>
+      <c r="O31" s="24"/>
+      <c r="P31" s="24"/>
+      <c r="Q31" s="13"/>
+    </row>
+    <row r="32" spans="4:17" ht="14.5" thickBot="1">
+      <c r="D32" s="17"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="15"/>
+      <c r="G32" s="14"/>
+      <c r="H32" s="14"/>
+      <c r="I32" s="14"/>
+      <c r="J32" s="14"/>
+      <c r="K32" s="14"/>
+      <c r="L32" s="14"/>
+      <c r="M32" s="14"/>
+      <c r="N32" s="14"/>
+      <c r="O32" s="14"/>
+      <c r="P32" s="14"/>
+      <c r="Q32" s="15"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="D9:F11"/>
+    <mergeCell ref="D12:F16"/>
+    <mergeCell ref="D17:F20"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B481C610-A988-4A92-888E-0DCC8C5D2554}">
+  <dimension ref="D5:Q39"/>
+  <sheetViews>
+    <sheetView topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N45" sqref="N45"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14"/>
+  <cols>
+    <col min="1" max="7" width="8.6640625" style="84"/>
+    <col min="8" max="8" width="11.75" style="84" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.58203125" style="84" customWidth="1"/>
+    <col min="10" max="10" width="12.33203125" style="84" customWidth="1"/>
+    <col min="11" max="11" width="14.25" style="84" customWidth="1"/>
+    <col min="12" max="12" width="11.75" style="84" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.08203125" style="84" customWidth="1"/>
+    <col min="14" max="14" width="14.1640625" style="84" customWidth="1"/>
+    <col min="15" max="15" width="14.58203125" style="84" customWidth="1"/>
+    <col min="16" max="16384" width="8.6640625" style="84"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="4:17" ht="14.5" thickBot="1"/>
+    <row r="6" spans="4:17">
+      <c r="D6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="11"/>
+    </row>
+    <row r="7" spans="4:17">
+      <c r="D7" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="12"/>
+      <c r="N7" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="O7" s="7"/>
+      <c r="P7" s="7"/>
+      <c r="Q7" s="13"/>
+    </row>
+    <row r="8" spans="4:17" ht="14.5" thickBot="1">
+      <c r="D8" s="8"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="14"/>
+      <c r="P8" s="14"/>
+      <c r="Q8" s="15"/>
+    </row>
+    <row r="9" spans="4:17">
+      <c r="D9" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="41"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="10"/>
+      <c r="O9" s="10"/>
+      <c r="P9" s="10"/>
+      <c r="Q9" s="11"/>
+    </row>
+    <row r="10" spans="4:17">
+      <c r="D10" s="43"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="45"/>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="24"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="12"/>
+      <c r="N10" s="12"/>
+      <c r="O10" s="12"/>
+      <c r="P10" s="12"/>
+      <c r="Q10" s="13"/>
+    </row>
+    <row r="11" spans="4:17" ht="14.5" thickBot="1">
+      <c r="D11" s="46"/>
+      <c r="E11" s="47"/>
+      <c r="F11" s="48"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="78"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="12"/>
+      <c r="O11" s="12"/>
+      <c r="P11" s="12"/>
+      <c r="Q11" s="13"/>
+    </row>
+    <row r="12" spans="4:17" ht="14.5" thickBot="1">
+      <c r="D12" s="40" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="41"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="24"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="12"/>
+      <c r="M12" s="12"/>
+      <c r="N12" s="12"/>
+      <c r="O12" s="12"/>
+      <c r="P12" s="12"/>
+      <c r="Q12" s="13"/>
+    </row>
+    <row r="13" spans="4:17">
+      <c r="D13" s="43"/>
+      <c r="E13" s="44"/>
+      <c r="F13" s="45"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="112" t="s">
+        <v>128</v>
+      </c>
+      <c r="I13" s="113"/>
+      <c r="J13" s="112" t="s">
+        <v>125</v>
+      </c>
+      <c r="K13" s="113"/>
+      <c r="L13" s="112" t="s">
+        <v>126</v>
+      </c>
+      <c r="M13" s="113"/>
+      <c r="N13" s="112" t="s">
+        <v>127</v>
+      </c>
+      <c r="O13" s="113"/>
+      <c r="P13" s="12"/>
+      <c r="Q13" s="13"/>
+    </row>
+    <row r="14" spans="4:17">
+      <c r="D14" s="43"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="45"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="95"/>
+      <c r="I14" s="107"/>
+      <c r="J14" s="88"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="16"/>
+      <c r="M14" s="13"/>
+      <c r="N14" s="16"/>
+      <c r="O14" s="110"/>
+      <c r="P14" s="12"/>
+      <c r="Q14" s="13"/>
+    </row>
+    <row r="15" spans="4:17">
+      <c r="D15" s="43"/>
+      <c r="E15" s="44"/>
+      <c r="F15" s="45"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="95"/>
+      <c r="I15" s="90"/>
+      <c r="J15" s="89"/>
+      <c r="K15" s="90"/>
+      <c r="L15" s="89"/>
+      <c r="M15" s="90"/>
+      <c r="N15" s="16"/>
+      <c r="O15" s="90"/>
+      <c r="P15" s="86"/>
+      <c r="Q15" s="13"/>
+    </row>
+    <row r="16" spans="4:17" ht="14.5" thickBot="1">
+      <c r="D16" s="46"/>
+      <c r="E16" s="47"/>
+      <c r="F16" s="48"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="95"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="16"/>
+      <c r="K16" s="13"/>
+      <c r="L16" s="16"/>
+      <c r="M16" s="13"/>
+      <c r="N16" s="16"/>
+      <c r="O16" s="35"/>
+      <c r="P16" s="24"/>
+      <c r="Q16" s="13"/>
+    </row>
+    <row r="17" spans="4:17">
+      <c r="D17" s="85" t="s">
+        <v>124</v>
+      </c>
+      <c r="E17" s="61"/>
+      <c r="F17" s="62"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="95"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="16"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="16"/>
+      <c r="M17" s="13"/>
+      <c r="N17" s="16"/>
+      <c r="O17" s="35"/>
+      <c r="P17" s="24"/>
+      <c r="Q17" s="13"/>
+    </row>
+    <row r="18" spans="4:17">
+      <c r="D18" s="63"/>
+      <c r="E18" s="64"/>
+      <c r="F18" s="65"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="95"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="16"/>
+      <c r="K18" s="13"/>
+      <c r="L18" s="16"/>
+      <c r="M18" s="13"/>
+      <c r="N18" s="16"/>
+      <c r="O18" s="35"/>
+      <c r="P18" s="24"/>
+      <c r="Q18" s="13"/>
+    </row>
+    <row r="19" spans="4:17">
+      <c r="D19" s="63"/>
+      <c r="E19" s="64"/>
+      <c r="F19" s="65"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="16"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="16"/>
+      <c r="K19" s="13"/>
+      <c r="L19" s="16"/>
+      <c r="M19" s="13"/>
+      <c r="N19" s="16"/>
+      <c r="O19" s="13"/>
+      <c r="P19" s="12"/>
+      <c r="Q19" s="13"/>
+    </row>
+    <row r="20" spans="4:17" ht="14.5" thickBot="1">
+      <c r="D20" s="66"/>
+      <c r="E20" s="67"/>
+      <c r="F20" s="68"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="88"/>
+      <c r="I20" s="107"/>
+      <c r="J20" s="88"/>
+      <c r="K20" s="109"/>
+      <c r="L20" s="16"/>
+      <c r="M20" s="91"/>
+      <c r="N20" s="16"/>
+      <c r="O20" s="13"/>
+      <c r="P20" s="12"/>
+      <c r="Q20" s="13"/>
+    </row>
+    <row r="21" spans="4:17">
+      <c r="D21" s="16"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="89"/>
+      <c r="I21" s="90"/>
+      <c r="J21" s="89"/>
+      <c r="K21" s="90"/>
+      <c r="L21" s="89"/>
+      <c r="M21" s="90"/>
+      <c r="N21" s="89"/>
+      <c r="O21" s="90"/>
+      <c r="P21" s="86"/>
+      <c r="Q21" s="13"/>
+    </row>
+    <row r="22" spans="4:17">
+      <c r="D22" s="16"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="16"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="16"/>
+      <c r="K22" s="13"/>
+      <c r="L22" s="16"/>
+      <c r="M22" s="13"/>
+      <c r="N22" s="16"/>
+      <c r="O22" s="13"/>
+      <c r="P22" s="12"/>
+      <c r="Q22" s="13"/>
+    </row>
+    <row r="23" spans="4:17">
+      <c r="D23" s="16"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="88"/>
+      <c r="I23" s="107"/>
+      <c r="J23" s="88"/>
+      <c r="K23" s="109"/>
+      <c r="L23" s="16"/>
+      <c r="M23" s="91"/>
+      <c r="N23" s="16"/>
+      <c r="O23" s="13"/>
+      <c r="P23" s="12"/>
+      <c r="Q23" s="13"/>
+    </row>
+    <row r="24" spans="4:17">
+      <c r="D24" s="16"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="89"/>
+      <c r="I24" s="90"/>
+      <c r="J24" s="89"/>
+      <c r="K24" s="90"/>
+      <c r="L24" s="89"/>
+      <c r="M24" s="90"/>
+      <c r="N24" s="89"/>
+      <c r="O24" s="90"/>
+      <c r="P24" s="86"/>
+      <c r="Q24" s="13"/>
+    </row>
+    <row r="25" spans="4:17">
+      <c r="D25" s="16"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="108"/>
+      <c r="I25" s="13"/>
+      <c r="J25" s="16"/>
+      <c r="K25" s="13"/>
+      <c r="L25" s="16"/>
+      <c r="M25" s="13"/>
+      <c r="N25" s="16"/>
+      <c r="O25" s="13"/>
+      <c r="P25" s="12"/>
+      <c r="Q25" s="13"/>
+    </row>
+    <row r="26" spans="4:17">
+      <c r="D26" s="16"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="108"/>
+      <c r="I26" s="35"/>
+      <c r="J26" s="108"/>
+      <c r="K26" s="35"/>
+      <c r="L26" s="108"/>
+      <c r="M26" s="13"/>
+      <c r="N26" s="16"/>
+      <c r="O26" s="35"/>
+      <c r="P26" s="24"/>
+      <c r="Q26" s="13"/>
+    </row>
+    <row r="27" spans="4:17" ht="14.5" thickBot="1">
+      <c r="D27" s="16"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="17"/>
+      <c r="I27" s="15"/>
+      <c r="J27" s="17"/>
+      <c r="K27" s="15"/>
+      <c r="L27" s="17"/>
+      <c r="M27" s="15"/>
+      <c r="N27" s="17"/>
+      <c r="O27" s="111"/>
+      <c r="P27" s="24"/>
+      <c r="Q27" s="13"/>
+    </row>
+    <row r="28" spans="4:17">
+      <c r="D28" s="16"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="69"/>
+      <c r="I28" s="69"/>
+      <c r="J28" s="69"/>
+      <c r="K28" s="12"/>
+      <c r="L28" s="12"/>
+      <c r="M28" s="12"/>
+      <c r="N28" s="12"/>
+      <c r="O28" s="24"/>
+      <c r="P28" s="24"/>
+      <c r="Q28" s="13"/>
+    </row>
+    <row r="29" spans="4:17" ht="14.5" thickBot="1">
+      <c r="D29" s="16"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="137" t="s">
+        <v>129</v>
+      </c>
+      <c r="I29" s="137"/>
+      <c r="J29" s="69"/>
+      <c r="K29" s="12"/>
+      <c r="L29" s="12"/>
+      <c r="M29" s="12"/>
+      <c r="N29" s="12"/>
+      <c r="O29" s="24"/>
+      <c r="P29" s="24"/>
+      <c r="Q29" s="13"/>
+    </row>
+    <row r="30" spans="4:17" ht="16" thickBot="1">
+      <c r="D30" s="16"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="135" t="s">
+        <v>128</v>
+      </c>
+      <c r="I30" s="136"/>
+      <c r="J30" s="135" t="s">
+        <v>125</v>
+      </c>
+      <c r="K30" s="136"/>
+      <c r="L30" s="135" t="s">
+        <v>126</v>
+      </c>
+      <c r="M30" s="136"/>
+      <c r="N30" s="135" t="s">
+        <v>127</v>
+      </c>
+      <c r="O30" s="136"/>
+      <c r="P30" s="24"/>
+      <c r="Q30" s="13"/>
+    </row>
+    <row r="31" spans="4:17" ht="14.5" thickBot="1">
+      <c r="D31" s="16"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="12"/>
+      <c r="H31" s="139" t="s">
+        <v>131</v>
+      </c>
+      <c r="I31" s="140" t="s">
+        <v>132</v>
+      </c>
+      <c r="J31" s="139" t="s">
+        <v>131</v>
+      </c>
+      <c r="K31" s="140" t="s">
+        <v>132</v>
+      </c>
+      <c r="L31" s="139" t="s">
+        <v>131</v>
+      </c>
+      <c r="M31" s="140" t="s">
+        <v>132</v>
+      </c>
+      <c r="N31" s="139" t="s">
+        <v>131</v>
+      </c>
+      <c r="O31" s="141" t="s">
+        <v>132</v>
+      </c>
+      <c r="P31" s="24"/>
+      <c r="Q31" s="13"/>
+    </row>
+    <row r="32" spans="4:17">
+      <c r="D32" s="16"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="12"/>
+      <c r="H32" s="138" t="s">
+        <v>130</v>
+      </c>
+      <c r="I32" s="142">
+        <v>40</v>
+      </c>
+      <c r="J32" s="114"/>
+      <c r="K32" s="10"/>
+      <c r="L32" s="10"/>
+      <c r="M32" s="10"/>
+      <c r="N32" s="10"/>
+      <c r="O32" s="115"/>
+      <c r="P32" s="24"/>
+      <c r="Q32" s="13"/>
+    </row>
+    <row r="33" spans="4:17">
+      <c r="D33" s="16"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="12"/>
+      <c r="H33" s="133" t="s">
+        <v>143</v>
+      </c>
+      <c r="I33" s="134">
+        <v>40.5</v>
+      </c>
+      <c r="J33" s="69"/>
+      <c r="K33" s="12"/>
+      <c r="L33" s="12"/>
+      <c r="M33" s="12"/>
+      <c r="N33" s="12"/>
+      <c r="O33" s="35"/>
+      <c r="P33" s="24"/>
+      <c r="Q33" s="13"/>
+    </row>
+    <row r="34" spans="4:17">
+      <c r="D34" s="16"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="13"/>
+      <c r="G34" s="12"/>
+      <c r="H34" s="133" t="s">
+        <v>144</v>
+      </c>
+      <c r="I34" s="134">
+        <v>39.6</v>
+      </c>
+      <c r="J34" s="80"/>
+      <c r="K34" s="80"/>
+      <c r="L34" s="80"/>
+      <c r="M34" s="80"/>
+      <c r="N34" s="80"/>
+      <c r="O34" s="99"/>
+      <c r="P34" s="80"/>
+      <c r="Q34" s="13"/>
+    </row>
+    <row r="35" spans="4:17" ht="14.5" thickBot="1">
+      <c r="D35" s="16"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="12"/>
+      <c r="H35" s="143" t="s">
+        <v>145</v>
+      </c>
+      <c r="I35" s="144">
+        <v>41</v>
+      </c>
+      <c r="J35" s="145"/>
+      <c r="K35" s="145"/>
+      <c r="L35" s="145"/>
+      <c r="M35" s="145"/>
+      <c r="N35" s="145"/>
+      <c r="O35" s="146"/>
+      <c r="P35" s="80"/>
+      <c r="Q35" s="13"/>
+    </row>
+    <row r="36" spans="4:17">
+      <c r="D36" s="16"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="12"/>
+      <c r="H36" s="98"/>
+      <c r="I36" s="80"/>
+      <c r="J36" s="80"/>
+      <c r="K36" s="80"/>
+      <c r="L36" s="80"/>
+      <c r="M36" s="80"/>
+      <c r="N36" s="80"/>
+      <c r="O36" s="99"/>
+      <c r="P36" s="80"/>
+      <c r="Q36" s="13"/>
+    </row>
+    <row r="37" spans="4:17" ht="14.5" thickBot="1">
+      <c r="D37" s="16"/>
+      <c r="E37" s="12"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="12"/>
+      <c r="H37" s="17"/>
+      <c r="I37" s="14"/>
+      <c r="J37" s="14"/>
+      <c r="K37" s="14"/>
+      <c r="L37" s="14"/>
+      <c r="M37" s="14"/>
+      <c r="N37" s="14"/>
+      <c r="O37" s="111"/>
+      <c r="P37" s="24"/>
+      <c r="Q37" s="13"/>
+    </row>
+    <row r="38" spans="4:17">
+      <c r="D38" s="16"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="13"/>
+      <c r="G38" s="12"/>
+      <c r="H38" s="12"/>
+      <c r="I38" s="12"/>
+      <c r="J38" s="12"/>
+      <c r="K38" s="12"/>
+      <c r="L38" s="12"/>
+      <c r="M38" s="12"/>
+      <c r="N38" s="12"/>
+      <c r="O38" s="24"/>
+      <c r="P38" s="24"/>
+      <c r="Q38" s="13"/>
+    </row>
+    <row r="39" spans="4:17" ht="14.5" thickBot="1">
+      <c r="D39" s="17"/>
+      <c r="E39" s="14"/>
+      <c r="F39" s="15"/>
+      <c r="G39" s="14"/>
+      <c r="H39" s="14"/>
+      <c r="I39" s="14"/>
+      <c r="J39" s="14"/>
+      <c r="K39" s="14"/>
+      <c r="L39" s="14"/>
+      <c r="M39" s="14"/>
+      <c r="N39" s="14"/>
+      <c r="O39" s="14"/>
+      <c r="P39" s="14"/>
+      <c r="Q39" s="15"/>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="N13:O13"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="L30:M30"/>
+    <mergeCell ref="N30:O30"/>
+    <mergeCell ref="D9:F11"/>
+    <mergeCell ref="D12:F16"/>
+    <mergeCell ref="D17:F20"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="L13:M13"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F50A82F-4F20-458B-9395-69DAEEAD96DD}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14"/>
+  <cols>
+    <col min="1" max="16384" width="8.6640625" style="59"/>
+  </cols>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[2018-10-30] Design document - update 2
</commit_message>
<xml_diff>
--- a/demo-design-doc/Feature List.xlsx
+++ b/demo-design-doc/Feature List.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{084612A2-3A99-43C7-AEFD-76B50442FF1C}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DC01651-5C0F-4ED8-BEF8-878DE58DFBE1}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" tabRatio="772" firstSheet="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" tabRatio="772" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -1413,6 +1413,58 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="15" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1506,73 +1558,21 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="12" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="4" fontId="4" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="15" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -2776,6 +2776,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-CFD8-40CE-84F9-06C438A7A471}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -2791,6 +2796,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-CFD8-40CE-84F9-06C438A7A471}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -2806,6 +2816,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-CFD8-40CE-84F9-06C438A7A471}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -2821,6 +2836,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-CFD8-40CE-84F9-06C438A7A471}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
@@ -7340,144 +7360,6 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>99787</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>136071</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>535215</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>136071</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="矩形: 圆角 7">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{906AC792-D364-4A9D-8345-D63F2F08884B}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="14006287" y="498928"/>
-          <a:ext cx="435428" cy="362857"/>
-        </a:xfrm>
-        <a:prstGeom prst="roundRect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="bg1"/>
-        </a:solidFill>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="en-US" altLang="zh-CN" sz="1600">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>7</a:t>
-          </a:r>
-          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1600">
-            <a:solidFill>
-              <a:srgbClr val="FF0000"/>
-            </a:solidFill>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>235858</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>90714</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>9072</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>136071</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="笑脸 5">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CF0B1337-4264-4DDD-B733-A0B68DA2DC3B}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="13480144" y="816428"/>
-          <a:ext cx="435428" cy="408214"/>
-        </a:xfrm>
-        <a:prstGeom prst="smileyFace">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>181429</xdr:colOff>
       <xdr:row>10</xdr:row>
@@ -9604,39 +9486,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="8.6640625" style="155"/>
-    <col min="2" max="2" width="10.4140625" style="155" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32" style="155" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25" style="155" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="8.6640625" style="155"/>
-    <col min="7" max="7" width="11.9140625" style="155" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.6640625" style="155"/>
+    <col min="1" max="1" width="8.6640625" style="119"/>
+    <col min="2" max="2" width="10.4140625" style="119" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32" style="119" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25" style="119" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="8.6640625" style="119"/>
+    <col min="7" max="7" width="11.9140625" style="119" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.6640625" style="119"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="155" t="s">
+      <c r="A1" s="119" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="155" t="s">
+      <c r="E1" s="119" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="155" t="s">
+      <c r="F1" s="119" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="B2" s="155" t="s">
+      <c r="B2" s="119" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="C3" s="155" t="s">
+      <c r="C3" s="119" t="s">
         <v>1</v>
       </c>
     </row>
@@ -9644,26 +9526,26 @@
       <c r="D4" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="156" t="s">
+      <c r="E4" s="120" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="155">
+      <c r="F4" s="119">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="D5" s="157" t="s">
+      <c r="D5" s="121" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="158" t="s">
+      <c r="E5" s="122" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="157">
+      <c r="F5" s="121">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="C6" s="155" t="s">
+      <c r="C6" s="119" t="s">
         <v>3</v>
       </c>
     </row>
@@ -9671,10 +9553,10 @@
       <c r="D7" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="156" t="s">
+      <c r="E7" s="120" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="155">
+      <c r="F7" s="119">
         <v>1</v>
       </c>
     </row>
@@ -9682,15 +9564,15 @@
       <c r="D8" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="156" t="s">
+      <c r="E8" s="120" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="155">
+      <c r="F8" s="119">
         <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="C9" s="155" t="s">
+      <c r="C9" s="119" t="s">
         <v>7</v>
       </c>
     </row>
@@ -9698,20 +9580,20 @@
       <c r="D10" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="156" t="s">
+      <c r="E10" s="120" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="155">
+      <c r="F10" s="119">
         <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="B13" s="155" t="s">
+      <c r="B13" s="119" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="C14" s="155" t="s">
+      <c r="C14" s="119" t="s">
         <v>11</v>
       </c>
     </row>
@@ -9719,15 +9601,15 @@
       <c r="D15" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="E15" s="156" t="s">
+      <c r="E15" s="120" t="s">
         <v>15</v>
       </c>
-      <c r="F15" s="155">
+      <c r="F15" s="119">
         <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="C16" s="155" t="s">
+      <c r="C16" s="119" t="s">
         <v>12</v>
       </c>
     </row>
@@ -9735,15 +9617,15 @@
       <c r="D17" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="E17" s="156" t="s">
+      <c r="E17" s="120" t="s">
         <v>15</v>
       </c>
-      <c r="F17" s="155">
+      <c r="F17" s="119">
         <v>4</v>
       </c>
     </row>
     <row r="18" spans="2:7">
-      <c r="C18" s="155" t="s">
+      <c r="C18" s="119" t="s">
         <v>14</v>
       </c>
     </row>
@@ -9751,10 +9633,10 @@
       <c r="D19" s="31" t="s">
         <v>106</v>
       </c>
-      <c r="E19" s="156" t="s">
+      <c r="E19" s="120" t="s">
         <v>15</v>
       </c>
-      <c r="F19" s="155">
+      <c r="F19" s="119">
         <v>5</v>
       </c>
     </row>
@@ -9762,28 +9644,28 @@
       <c r="D20" s="31" t="s">
         <v>143</v>
       </c>
-      <c r="E20" s="156" t="s">
+      <c r="E20" s="120" t="s">
         <v>15</v>
       </c>
-      <c r="F20" s="155">
+      <c r="F20" s="119">
         <v>20</v>
       </c>
-      <c r="G20" s="155" t="s">
+      <c r="G20" s="119" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="21" spans="2:7">
-      <c r="C21" s="155" t="s">
+      <c r="C21" s="119" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="23" spans="2:7">
-      <c r="B23" s="155" t="s">
+      <c r="B23" s="119" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="24" spans="2:7">
-      <c r="C24" s="155" t="s">
+      <c r="C24" s="119" t="s">
         <v>153</v>
       </c>
     </row>
@@ -9791,10 +9673,10 @@
       <c r="D25" s="31" t="s">
         <v>154</v>
       </c>
-      <c r="E25" s="156" t="s">
+      <c r="E25" s="120" t="s">
         <v>166</v>
       </c>
-      <c r="F25" s="155">
+      <c r="F25" s="119">
         <v>10</v>
       </c>
     </row>
@@ -9850,7 +9732,7 @@
       <c r="M5" s="3"/>
       <c r="N5" s="3"/>
       <c r="O5" s="8"/>
-      <c r="P5" s="146"/>
+      <c r="P5" s="110"/>
       <c r="Q5" s="3"/>
       <c r="R5" s="3"/>
       <c r="S5" s="3" t="s">
@@ -9873,7 +9755,7 @@
       <c r="M6" s="5"/>
       <c r="N6" s="5"/>
       <c r="O6" s="10"/>
-      <c r="P6" s="147"/>
+      <c r="P6" s="111"/>
       <c r="Q6" s="5"/>
       <c r="R6" s="5"/>
       <c r="S6" s="5" t="s">
@@ -9902,11 +9784,11 @@
       <c r="U7" s="13"/>
     </row>
     <row r="8" spans="5:21" ht="14" customHeight="1">
-      <c r="E8" s="128" t="s">
+      <c r="E8" s="156" t="s">
         <v>155</v>
       </c>
-      <c r="F8" s="120"/>
-      <c r="G8" s="121"/>
+      <c r="F8" s="148"/>
+      <c r="G8" s="149"/>
       <c r="H8" s="21"/>
       <c r="I8" s="21"/>
       <c r="J8" s="8"/>
@@ -9923,9 +9805,9 @@
       <c r="U8" s="9"/>
     </row>
     <row r="9" spans="5:21">
-      <c r="E9" s="122"/>
-      <c r="F9" s="123"/>
-      <c r="G9" s="124"/>
+      <c r="E9" s="150"/>
+      <c r="F9" s="151"/>
+      <c r="G9" s="152"/>
       <c r="H9" s="22"/>
       <c r="I9" s="22"/>
       <c r="J9" s="22"/>
@@ -9942,9 +9824,9 @@
       <c r="U9" s="11"/>
     </row>
     <row r="10" spans="5:21" ht="14.5" thickBot="1">
-      <c r="E10" s="122"/>
-      <c r="F10" s="123"/>
-      <c r="G10" s="124"/>
+      <c r="E10" s="150"/>
+      <c r="F10" s="151"/>
+      <c r="G10" s="152"/>
       <c r="H10" s="10"/>
       <c r="I10" s="10"/>
       <c r="J10" s="10"/>
@@ -9961,9 +9843,9 @@
       <c r="U10" s="11"/>
     </row>
     <row r="11" spans="5:21">
-      <c r="E11" s="100"/>
-      <c r="F11" s="101"/>
-      <c r="G11" s="102"/>
+      <c r="E11" s="128"/>
+      <c r="F11" s="129"/>
+      <c r="G11" s="130"/>
       <c r="H11" s="22"/>
       <c r="I11" s="10"/>
       <c r="J11" s="10"/>
@@ -9980,37 +9862,37 @@
       <c r="U11" s="11"/>
     </row>
     <row r="12" spans="5:21">
-      <c r="E12" s="103"/>
-      <c r="F12" s="104"/>
-      <c r="G12" s="105"/>
+      <c r="E12" s="131"/>
+      <c r="F12" s="132"/>
+      <c r="G12" s="133"/>
       <c r="H12" s="22"/>
       <c r="I12" s="54" t="s">
         <v>156</v>
       </c>
-      <c r="J12" s="161" t="s">
+      <c r="J12" s="125" t="s">
         <v>159</v>
       </c>
-      <c r="K12" s="159"/>
-      <c r="L12" s="144"/>
-      <c r="M12" s="144"/>
-      <c r="N12" s="144"/>
-      <c r="O12" s="144"/>
-      <c r="P12" s="144"/>
-      <c r="Q12" s="144"/>
+      <c r="K12" s="123"/>
+      <c r="L12" s="159"/>
+      <c r="M12" s="159"/>
+      <c r="N12" s="159"/>
+      <c r="O12" s="159"/>
+      <c r="P12" s="159"/>
+      <c r="Q12" s="159"/>
       <c r="R12" s="10"/>
       <c r="S12" s="10"/>
       <c r="T12" s="10"/>
       <c r="U12" s="11"/>
     </row>
     <row r="13" spans="5:21">
-      <c r="E13" s="103"/>
-      <c r="F13" s="104"/>
-      <c r="G13" s="105"/>
+      <c r="E13" s="131"/>
+      <c r="F13" s="132"/>
+      <c r="G13" s="133"/>
       <c r="H13" s="22"/>
       <c r="I13" s="54" t="s">
         <v>157</v>
       </c>
-      <c r="J13" s="160" t="s">
+      <c r="J13" s="124" t="s">
         <v>160</v>
       </c>
       <c r="K13" s="40"/>
@@ -10026,14 +9908,14 @@
       <c r="U13" s="11"/>
     </row>
     <row r="14" spans="5:21">
-      <c r="E14" s="103"/>
-      <c r="F14" s="104"/>
-      <c r="G14" s="105"/>
+      <c r="E14" s="131"/>
+      <c r="F14" s="132"/>
+      <c r="G14" s="133"/>
       <c r="H14" s="10"/>
       <c r="I14" s="54" t="s">
         <v>158</v>
       </c>
-      <c r="J14" s="160" t="s">
+      <c r="J14" s="124" t="s">
         <v>161</v>
       </c>
       <c r="K14" s="56"/>
@@ -10049,14 +9931,14 @@
       <c r="U14" s="11"/>
     </row>
     <row r="15" spans="5:21" ht="14.5" thickBot="1">
-      <c r="E15" s="106"/>
-      <c r="F15" s="107"/>
-      <c r="G15" s="108"/>
+      <c r="E15" s="134"/>
+      <c r="F15" s="135"/>
+      <c r="G15" s="136"/>
       <c r="H15" s="10"/>
       <c r="I15" s="54" t="s">
         <v>162</v>
       </c>
-      <c r="J15" s="160" t="s">
+      <c r="J15" s="124" t="s">
         <v>163</v>
       </c>
       <c r="K15" s="10"/>
@@ -10072,14 +9954,14 @@
       <c r="U15" s="11"/>
     </row>
     <row r="16" spans="5:21">
-      <c r="E16" s="142"/>
-      <c r="F16" s="101"/>
-      <c r="G16" s="102"/>
+      <c r="E16" s="163"/>
+      <c r="F16" s="129"/>
+      <c r="G16" s="130"/>
       <c r="H16" s="10"/>
       <c r="I16" s="54" t="s">
         <v>164</v>
       </c>
-      <c r="J16" s="160" t="s">
+      <c r="J16" s="124" t="s">
         <v>165</v>
       </c>
       <c r="K16" s="10"/>
@@ -10095,9 +9977,9 @@
       <c r="U16" s="11"/>
     </row>
     <row r="17" spans="5:21">
-      <c r="E17" s="103"/>
-      <c r="F17" s="104"/>
-      <c r="G17" s="105"/>
+      <c r="E17" s="131"/>
+      <c r="F17" s="132"/>
+      <c r="G17" s="133"/>
       <c r="H17" s="10"/>
       <c r="I17" s="10"/>
       <c r="L17" s="10"/>
@@ -10112,9 +9994,9 @@
       <c r="U17" s="11"/>
     </row>
     <row r="18" spans="5:21">
-      <c r="E18" s="103"/>
-      <c r="F18" s="104"/>
-      <c r="G18" s="105"/>
+      <c r="E18" s="131"/>
+      <c r="F18" s="132"/>
+      <c r="G18" s="133"/>
       <c r="H18" s="10"/>
       <c r="I18" s="10"/>
       <c r="J18" s="10"/>
@@ -10131,9 +10013,9 @@
       <c r="U18" s="11"/>
     </row>
     <row r="19" spans="5:21" ht="14.5" thickBot="1">
-      <c r="E19" s="106"/>
-      <c r="F19" s="107"/>
-      <c r="G19" s="108"/>
+      <c r="E19" s="134"/>
+      <c r="F19" s="135"/>
+      <c r="G19" s="136"/>
       <c r="H19" s="10"/>
       <c r="I19" s="10"/>
       <c r="J19" s="40"/>
@@ -10232,19 +10114,19 @@
       <c r="F24" s="10"/>
       <c r="G24" s="11"/>
       <c r="H24" s="10"/>
-      <c r="I24" s="162" t="s">
+      <c r="I24" s="126" t="s">
         <v>156</v>
       </c>
-      <c r="J24" s="162" t="s">
+      <c r="J24" s="126" t="s">
         <v>157</v>
       </c>
-      <c r="K24" s="162" t="s">
+      <c r="K24" s="126" t="s">
         <v>158</v>
       </c>
-      <c r="L24" s="162" t="s">
+      <c r="L24" s="126" t="s">
         <v>162</v>
       </c>
-      <c r="M24" s="162" t="s">
+      <c r="M24" s="126" t="s">
         <v>164</v>
       </c>
       <c r="N24" s="10"/>
@@ -10299,10 +10181,10 @@
       <c r="K26" s="53" t="s">
         <v>173</v>
       </c>
-      <c r="L26" s="163" t="s">
+      <c r="L26" s="127" t="s">
         <v>174</v>
       </c>
-      <c r="M26" s="163" t="s">
+      <c r="M26" s="127" t="s">
         <v>174</v>
       </c>
       <c r="N26" s="10"/>
@@ -10358,14 +10240,14 @@
       <c r="G29" s="11"/>
       <c r="H29" s="10"/>
       <c r="I29" s="10"/>
-      <c r="J29" s="145"/>
-      <c r="K29" s="145"/>
-      <c r="L29" s="145"/>
-      <c r="M29" s="145"/>
-      <c r="N29" s="145"/>
-      <c r="O29" s="145"/>
-      <c r="P29" s="145"/>
-      <c r="Q29" s="145"/>
+      <c r="J29" s="162"/>
+      <c r="K29" s="162"/>
+      <c r="L29" s="162"/>
+      <c r="M29" s="162"/>
+      <c r="N29" s="162"/>
+      <c r="O29" s="162"/>
+      <c r="P29" s="162"/>
+      <c r="Q29" s="162"/>
       <c r="R29" s="22"/>
       <c r="S29" s="22"/>
       <c r="T29" s="22"/>
@@ -10544,16 +10426,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="E8:G10"/>
+    <mergeCell ref="E11:G15"/>
+    <mergeCell ref="L12:M12"/>
+    <mergeCell ref="N12:O12"/>
+    <mergeCell ref="P12:Q12"/>
     <mergeCell ref="E16:G19"/>
     <mergeCell ref="J29:K29"/>
     <mergeCell ref="L29:M29"/>
     <mergeCell ref="N29:O29"/>
     <mergeCell ref="P29:Q29"/>
-    <mergeCell ref="E8:G10"/>
-    <mergeCell ref="E11:G15"/>
-    <mergeCell ref="L12:M12"/>
-    <mergeCell ref="N12:O12"/>
-    <mergeCell ref="P12:Q12"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10628,11 +10510,11 @@
       <c r="N5" s="13"/>
     </row>
     <row r="6" spans="4:14">
-      <c r="D6" s="100" t="s">
+      <c r="D6" s="128" t="s">
         <v>1</v>
       </c>
-      <c r="E6" s="101"/>
-      <c r="F6" s="102"/>
+      <c r="E6" s="129"/>
+      <c r="F6" s="130"/>
       <c r="G6" s="21" t="s">
         <v>23</v>
       </c>
@@ -10651,9 +10533,9 @@
       <c r="N6" s="9"/>
     </row>
     <row r="7" spans="4:14">
-      <c r="D7" s="103"/>
-      <c r="E7" s="104"/>
-      <c r="F7" s="105"/>
+      <c r="D7" s="131"/>
+      <c r="E7" s="132"/>
+      <c r="F7" s="133"/>
       <c r="G7" s="22" t="s">
         <v>29</v>
       </c>
@@ -10670,9 +10552,9 @@
       <c r="N7" s="11"/>
     </row>
     <row r="8" spans="4:14" ht="14.5" thickBot="1">
-      <c r="D8" s="106"/>
-      <c r="E8" s="107"/>
-      <c r="F8" s="108"/>
+      <c r="D8" s="134"/>
+      <c r="E8" s="135"/>
+      <c r="F8" s="136"/>
       <c r="G8" s="22" t="s">
         <v>32</v>
       </c>
@@ -10691,11 +10573,11 @@
       <c r="N8" s="11"/>
     </row>
     <row r="9" spans="4:14">
-      <c r="D9" s="109" t="s">
+      <c r="D9" s="137" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="110"/>
-      <c r="F9" s="111"/>
+      <c r="E9" s="138"/>
+      <c r="F9" s="139"/>
       <c r="G9" s="27" t="s">
         <v>35</v>
       </c>
@@ -10710,9 +10592,9 @@
       <c r="N9" s="17"/>
     </row>
     <row r="10" spans="4:14">
-      <c r="D10" s="112"/>
-      <c r="E10" s="113"/>
-      <c r="F10" s="114"/>
+      <c r="D10" s="140"/>
+      <c r="E10" s="141"/>
+      <c r="F10" s="142"/>
       <c r="G10" s="10"/>
       <c r="H10" s="10"/>
       <c r="I10" s="10"/>
@@ -10723,9 +10605,9 @@
       <c r="N10" s="11"/>
     </row>
     <row r="11" spans="4:14">
-      <c r="D11" s="112"/>
-      <c r="E11" s="113"/>
-      <c r="F11" s="114"/>
+      <c r="D11" s="140"/>
+      <c r="E11" s="141"/>
+      <c r="F11" s="142"/>
       <c r="G11" s="10"/>
       <c r="H11" s="10"/>
       <c r="I11" s="10"/>
@@ -10736,9 +10618,9 @@
       <c r="N11" s="11"/>
     </row>
     <row r="12" spans="4:14" ht="14.5" thickBot="1">
-      <c r="D12" s="115"/>
-      <c r="E12" s="116"/>
-      <c r="F12" s="117"/>
+      <c r="D12" s="143"/>
+      <c r="E12" s="144"/>
+      <c r="F12" s="145"/>
       <c r="G12" s="10"/>
       <c r="H12" s="10"/>
       <c r="I12" s="10"/>
@@ -10753,11 +10635,11 @@
       <c r="N12" s="11"/>
     </row>
     <row r="13" spans="4:14">
-      <c r="D13" s="100" t="s">
+      <c r="D13" s="128" t="s">
         <v>34</v>
       </c>
-      <c r="E13" s="101"/>
-      <c r="F13" s="102"/>
+      <c r="E13" s="129"/>
+      <c r="F13" s="130"/>
       <c r="G13" s="10"/>
       <c r="H13" s="10"/>
       <c r="I13" s="10"/>
@@ -10772,9 +10654,9 @@
       <c r="N13" s="11"/>
     </row>
     <row r="14" spans="4:14">
-      <c r="D14" s="103"/>
-      <c r="E14" s="104"/>
-      <c r="F14" s="105"/>
+      <c r="D14" s="131"/>
+      <c r="E14" s="132"/>
+      <c r="F14" s="133"/>
       <c r="G14" s="10"/>
       <c r="H14" s="10"/>
       <c r="I14" s="10"/>
@@ -10789,9 +10671,9 @@
       <c r="N14" s="11"/>
     </row>
     <row r="15" spans="4:14">
-      <c r="D15" s="103"/>
-      <c r="E15" s="104"/>
-      <c r="F15" s="105"/>
+      <c r="D15" s="131"/>
+      <c r="E15" s="132"/>
+      <c r="F15" s="133"/>
       <c r="G15" s="10"/>
       <c r="H15" s="10"/>
       <c r="I15" s="10"/>
@@ -10806,9 +10688,9 @@
       <c r="N15" s="11"/>
     </row>
     <row r="16" spans="4:14" ht="14.5" thickBot="1">
-      <c r="D16" s="106"/>
-      <c r="E16" s="107"/>
-      <c r="F16" s="108"/>
+      <c r="D16" s="134"/>
+      <c r="E16" s="135"/>
+      <c r="F16" s="136"/>
       <c r="G16" s="10"/>
       <c r="H16" s="10"/>
       <c r="I16" s="10"/>
@@ -10961,11 +10843,11 @@
       <c r="N5" s="13"/>
     </row>
     <row r="6" spans="4:14">
-      <c r="D6" s="100" t="s">
+      <c r="D6" s="128" t="s">
         <v>1</v>
       </c>
-      <c r="E6" s="101"/>
-      <c r="F6" s="102"/>
+      <c r="E6" s="129"/>
+      <c r="F6" s="130"/>
       <c r="G6" s="21" t="s">
         <v>46</v>
       </c>
@@ -10986,9 +10868,9 @@
       <c r="N6" s="9"/>
     </row>
     <row r="7" spans="4:14">
-      <c r="D7" s="103"/>
-      <c r="E7" s="104"/>
-      <c r="F7" s="105"/>
+      <c r="D7" s="131"/>
+      <c r="E7" s="132"/>
+      <c r="F7" s="133"/>
       <c r="G7" s="22" t="s">
         <v>23</v>
       </c>
@@ -11007,9 +10889,9 @@
       <c r="N7" s="11"/>
     </row>
     <row r="8" spans="4:14" ht="14.5" thickBot="1">
-      <c r="D8" s="106"/>
-      <c r="E8" s="107"/>
-      <c r="F8" s="108"/>
+      <c r="D8" s="134"/>
+      <c r="E8" s="135"/>
+      <c r="F8" s="136"/>
       <c r="G8" s="22" t="s">
         <v>48</v>
       </c>
@@ -11030,11 +10912,11 @@
       <c r="N8" s="11"/>
     </row>
     <row r="9" spans="4:14">
-      <c r="D9" s="100" t="s">
+      <c r="D9" s="128" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="101"/>
-      <c r="F9" s="102"/>
+      <c r="E9" s="129"/>
+      <c r="F9" s="130"/>
       <c r="G9" s="27" t="s">
         <v>53</v>
       </c>
@@ -11055,9 +10937,9 @@
       <c r="N9" s="17"/>
     </row>
     <row r="10" spans="4:14">
-      <c r="D10" s="103"/>
-      <c r="E10" s="104"/>
-      <c r="F10" s="105"/>
+      <c r="D10" s="131"/>
+      <c r="E10" s="132"/>
+      <c r="F10" s="133"/>
       <c r="G10" s="10"/>
       <c r="H10" s="10"/>
       <c r="I10" s="10"/>
@@ -11068,9 +10950,9 @@
       <c r="N10" s="11"/>
     </row>
     <row r="11" spans="4:14">
-      <c r="D11" s="103"/>
-      <c r="E11" s="104"/>
-      <c r="F11" s="105"/>
+      <c r="D11" s="131"/>
+      <c r="E11" s="132"/>
+      <c r="F11" s="133"/>
       <c r="G11" s="10"/>
       <c r="H11" s="10"/>
       <c r="I11" s="10"/>
@@ -11081,9 +10963,9 @@
       <c r="N11" s="11"/>
     </row>
     <row r="12" spans="4:14" ht="14.5" thickBot="1">
-      <c r="D12" s="106"/>
-      <c r="E12" s="107"/>
-      <c r="F12" s="108"/>
+      <c r="D12" s="134"/>
+      <c r="E12" s="135"/>
+      <c r="F12" s="136"/>
       <c r="G12" s="10"/>
       <c r="H12" s="10"/>
       <c r="I12" s="10"/>
@@ -11098,11 +10980,11 @@
       <c r="N12" s="11"/>
     </row>
     <row r="13" spans="4:14">
-      <c r="D13" s="109" t="s">
+      <c r="D13" s="137" t="s">
         <v>34</v>
       </c>
-      <c r="E13" s="110"/>
-      <c r="F13" s="111"/>
+      <c r="E13" s="138"/>
+      <c r="F13" s="139"/>
       <c r="G13" s="10"/>
       <c r="H13" s="10"/>
       <c r="I13" s="10"/>
@@ -11117,9 +10999,9 @@
       <c r="N13" s="11"/>
     </row>
     <row r="14" spans="4:14">
-      <c r="D14" s="112"/>
-      <c r="E14" s="113"/>
-      <c r="F14" s="114"/>
+      <c r="D14" s="140"/>
+      <c r="E14" s="141"/>
+      <c r="F14" s="142"/>
       <c r="G14" s="10"/>
       <c r="H14" s="10"/>
       <c r="I14" s="10"/>
@@ -11134,9 +11016,9 @@
       <c r="N14" s="11"/>
     </row>
     <row r="15" spans="4:14">
-      <c r="D15" s="112"/>
-      <c r="E15" s="113"/>
-      <c r="F15" s="114"/>
+      <c r="D15" s="140"/>
+      <c r="E15" s="141"/>
+      <c r="F15" s="142"/>
       <c r="G15" s="10"/>
       <c r="H15" s="10"/>
       <c r="I15" s="10"/>
@@ -11151,9 +11033,9 @@
       <c r="N15" s="11"/>
     </row>
     <row r="16" spans="4:14" ht="14.5" thickBot="1">
-      <c r="D16" s="115"/>
-      <c r="E16" s="116"/>
-      <c r="F16" s="117"/>
+      <c r="D16" s="143"/>
+      <c r="E16" s="144"/>
+      <c r="F16" s="145"/>
       <c r="G16" s="10"/>
       <c r="H16" s="10"/>
       <c r="I16" s="10"/>
@@ -11306,11 +11188,11 @@
       <c r="N5" s="13"/>
     </row>
     <row r="6" spans="4:14">
-      <c r="D6" s="100" t="s">
+      <c r="D6" s="128" t="s">
         <v>1</v>
       </c>
-      <c r="E6" s="101"/>
-      <c r="F6" s="102"/>
+      <c r="E6" s="129"/>
+      <c r="F6" s="130"/>
       <c r="G6" s="21"/>
       <c r="H6" s="10"/>
       <c r="I6" s="10"/>
@@ -11321,9 +11203,9 @@
       <c r="N6" s="9"/>
     </row>
     <row r="7" spans="4:14">
-      <c r="D7" s="103"/>
-      <c r="E7" s="104"/>
-      <c r="F7" s="105"/>
+      <c r="D7" s="131"/>
+      <c r="E7" s="132"/>
+      <c r="F7" s="133"/>
       <c r="G7" s="22"/>
       <c r="H7" s="10"/>
       <c r="I7" s="10"/>
@@ -11334,9 +11216,9 @@
       <c r="N7" s="11"/>
     </row>
     <row r="8" spans="4:14" ht="14.5" thickBot="1">
-      <c r="D8" s="106"/>
-      <c r="E8" s="107"/>
-      <c r="F8" s="108"/>
+      <c r="D8" s="134"/>
+      <c r="E8" s="135"/>
+      <c r="F8" s="136"/>
       <c r="G8" s="22"/>
       <c r="H8" s="10"/>
       <c r="I8" s="10"/>
@@ -11347,11 +11229,11 @@
       <c r="N8" s="11"/>
     </row>
     <row r="9" spans="4:14">
-      <c r="D9" s="118" t="s">
+      <c r="D9" s="146" t="s">
         <v>65</v>
       </c>
-      <c r="E9" s="110"/>
-      <c r="F9" s="111"/>
+      <c r="E9" s="138"/>
+      <c r="F9" s="139"/>
       <c r="G9" s="32"/>
       <c r="H9" s="16"/>
       <c r="I9" s="16"/>
@@ -11362,9 +11244,9 @@
       <c r="N9" s="17"/>
     </row>
     <row r="10" spans="4:14">
-      <c r="D10" s="112"/>
-      <c r="E10" s="113"/>
-      <c r="F10" s="114"/>
+      <c r="D10" s="140"/>
+      <c r="E10" s="141"/>
+      <c r="F10" s="142"/>
       <c r="G10" s="10"/>
       <c r="H10" s="10"/>
       <c r="I10" s="10"/>
@@ -11379,9 +11261,9 @@
       </c>
     </row>
     <row r="11" spans="4:14">
-      <c r="D11" s="112"/>
-      <c r="E11" s="113"/>
-      <c r="F11" s="114"/>
+      <c r="D11" s="140"/>
+      <c r="E11" s="141"/>
+      <c r="F11" s="142"/>
       <c r="G11" s="10"/>
       <c r="H11" s="10"/>
       <c r="I11" s="10"/>
@@ -11396,9 +11278,9 @@
       </c>
     </row>
     <row r="12" spans="4:14" ht="14.5" thickBot="1">
-      <c r="D12" s="115"/>
-      <c r="E12" s="116"/>
-      <c r="F12" s="117"/>
+      <c r="D12" s="143"/>
+      <c r="E12" s="144"/>
+      <c r="F12" s="145"/>
       <c r="G12" s="10"/>
       <c r="H12" s="10"/>
       <c r="I12" s="10"/>
@@ -11413,11 +11295,11 @@
       </c>
     </row>
     <row r="13" spans="4:14">
-      <c r="D13" s="100" t="s">
+      <c r="D13" s="128" t="s">
         <v>34</v>
       </c>
-      <c r="E13" s="101"/>
-      <c r="F13" s="102"/>
+      <c r="E13" s="129"/>
+      <c r="F13" s="130"/>
       <c r="G13" s="10"/>
       <c r="H13" s="10"/>
       <c r="I13" s="10"/>
@@ -11432,9 +11314,9 @@
       </c>
     </row>
     <row r="14" spans="4:14">
-      <c r="D14" s="103"/>
-      <c r="E14" s="104"/>
-      <c r="F14" s="105"/>
+      <c r="D14" s="131"/>
+      <c r="E14" s="132"/>
+      <c r="F14" s="133"/>
       <c r="G14" s="10"/>
       <c r="H14" s="10"/>
       <c r="I14" s="10"/>
@@ -11449,9 +11331,9 @@
       </c>
     </row>
     <row r="15" spans="4:14">
-      <c r="D15" s="103"/>
-      <c r="E15" s="104"/>
-      <c r="F15" s="105"/>
+      <c r="D15" s="131"/>
+      <c r="E15" s="132"/>
+      <c r="F15" s="133"/>
       <c r="G15" s="10"/>
       <c r="H15" s="10"/>
       <c r="I15" s="10"/>
@@ -11466,9 +11348,9 @@
       </c>
     </row>
     <row r="16" spans="4:14" ht="14.5" thickBot="1">
-      <c r="D16" s="106"/>
-      <c r="E16" s="107"/>
-      <c r="F16" s="108"/>
+      <c r="D16" s="134"/>
+      <c r="E16" s="135"/>
+      <c r="F16" s="136"/>
       <c r="G16" s="10"/>
       <c r="H16" s="10"/>
       <c r="I16" s="10"/>
@@ -11621,11 +11503,11 @@
       <c r="O5" s="13"/>
     </row>
     <row r="6" spans="4:15">
-      <c r="D6" s="100" t="s">
+      <c r="D6" s="128" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="101"/>
-      <c r="F6" s="102"/>
+      <c r="E6" s="129"/>
+      <c r="F6" s="130"/>
       <c r="G6" s="21"/>
       <c r="H6" s="8"/>
       <c r="I6" s="8"/>
@@ -11637,9 +11519,9 @@
       <c r="O6" s="9"/>
     </row>
     <row r="7" spans="4:15">
-      <c r="D7" s="103"/>
-      <c r="E7" s="104"/>
-      <c r="F7" s="105"/>
+      <c r="D7" s="131"/>
+      <c r="E7" s="132"/>
+      <c r="F7" s="133"/>
       <c r="G7" s="22"/>
       <c r="H7" s="10"/>
       <c r="I7" s="10"/>
@@ -11651,9 +11533,9 @@
       <c r="O7" s="11"/>
     </row>
     <row r="8" spans="4:15" ht="14.5" thickBot="1">
-      <c r="D8" s="106"/>
-      <c r="E8" s="107"/>
-      <c r="F8" s="108"/>
+      <c r="D8" s="134"/>
+      <c r="E8" s="135"/>
+      <c r="F8" s="136"/>
       <c r="K8" s="10"/>
       <c r="L8" s="10"/>
       <c r="M8" s="10"/>
@@ -11661,11 +11543,11 @@
       <c r="O8" s="11"/>
     </row>
     <row r="9" spans="4:15">
-      <c r="D9" s="119" t="s">
+      <c r="D9" s="147" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="120"/>
-      <c r="F9" s="121"/>
+      <c r="E9" s="148"/>
+      <c r="F9" s="149"/>
       <c r="G9" s="22"/>
       <c r="K9" s="10"/>
       <c r="L9" s="10"/>
@@ -11674,9 +11556,9 @@
       <c r="O9" s="11"/>
     </row>
     <row r="10" spans="4:15">
-      <c r="D10" s="122"/>
-      <c r="E10" s="123"/>
-      <c r="F10" s="124"/>
+      <c r="D10" s="150"/>
+      <c r="E10" s="151"/>
+      <c r="F10" s="152"/>
       <c r="G10" s="10"/>
       <c r="H10" s="42" t="s">
         <v>68</v>
@@ -11702,20 +11584,20 @@
       <c r="O10" s="11"/>
     </row>
     <row r="11" spans="4:15">
-      <c r="D11" s="122"/>
-      <c r="E11" s="123"/>
-      <c r="F11" s="124"/>
+      <c r="D11" s="150"/>
+      <c r="E11" s="151"/>
+      <c r="F11" s="152"/>
       <c r="G11" s="10"/>
-      <c r="H11" s="141" t="s">
+      <c r="H11" s="108" t="s">
         <v>71</v>
       </c>
       <c r="I11" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="J11" s="139">
+      <c r="J11" s="106">
         <v>16300508.050000001</v>
       </c>
-      <c r="K11" s="139">
+      <c r="K11" s="106">
         <v>16300508.050000001</v>
       </c>
       <c r="L11" s="41">
@@ -11730,18 +11612,18 @@
       <c r="O11" s="11"/>
     </row>
     <row r="12" spans="4:15">
-      <c r="D12" s="122"/>
-      <c r="E12" s="123"/>
-      <c r="F12" s="124"/>
+      <c r="D12" s="150"/>
+      <c r="E12" s="151"/>
+      <c r="F12" s="152"/>
       <c r="G12" s="10"/>
       <c r="H12" s="10" t="s">
         <v>148</v>
       </c>
       <c r="I12" s="10"/>
-      <c r="J12" s="139">
+      <c r="J12" s="106">
         <v>5000300</v>
       </c>
-      <c r="K12" s="139">
+      <c r="K12" s="106">
         <v>0</v>
       </c>
       <c r="L12" s="41">
@@ -11757,18 +11639,18 @@
       <c r="O12" s="11"/>
     </row>
     <row r="13" spans="4:15">
-      <c r="D13" s="122"/>
-      <c r="E13" s="123"/>
-      <c r="F13" s="124"/>
+      <c r="D13" s="150"/>
+      <c r="E13" s="151"/>
+      <c r="F13" s="152"/>
       <c r="G13" s="10"/>
       <c r="H13" s="10" t="s">
         <v>149</v>
       </c>
       <c r="I13" s="10"/>
-      <c r="J13" s="139">
+      <c r="J13" s="106">
         <v>0</v>
       </c>
-      <c r="K13" s="139">
+      <c r="K13" s="106">
         <v>100000</v>
       </c>
       <c r="L13" s="41">
@@ -11784,18 +11666,18 @@
       <c r="O13" s="11"/>
     </row>
     <row r="14" spans="4:15" ht="14.5" thickBot="1">
-      <c r="D14" s="125"/>
-      <c r="E14" s="126"/>
-      <c r="F14" s="127"/>
+      <c r="D14" s="153"/>
+      <c r="E14" s="154"/>
+      <c r="F14" s="155"/>
       <c r="G14" s="10"/>
       <c r="H14" s="10" t="s">
         <v>150</v>
       </c>
       <c r="I14" s="10"/>
-      <c r="J14" s="139">
+      <c r="J14" s="106">
         <v>0</v>
       </c>
-      <c r="K14" s="139">
+      <c r="K14" s="106">
         <v>300000</v>
       </c>
       <c r="L14" s="41">
@@ -11811,11 +11693,11 @@
       <c r="O14" s="11"/>
     </row>
     <row r="15" spans="4:15">
-      <c r="D15" s="100" t="s">
+      <c r="D15" s="128" t="s">
         <v>67</v>
       </c>
-      <c r="E15" s="101"/>
-      <c r="F15" s="102"/>
+      <c r="E15" s="129"/>
+      <c r="F15" s="130"/>
       <c r="G15" s="10"/>
       <c r="H15" s="10" t="s">
         <v>74</v>
@@ -11823,10 +11705,10 @@
       <c r="I15" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="J15" s="139">
+      <c r="J15" s="106">
         <v>9789644.9800000004</v>
       </c>
-      <c r="K15" s="139">
+      <c r="K15" s="106">
         <v>9789644.9800000004</v>
       </c>
       <c r="L15" s="41">
@@ -11841,9 +11723,9 @@
       <c r="O15" s="11"/>
     </row>
     <row r="16" spans="4:15">
-      <c r="D16" s="103"/>
-      <c r="E16" s="104"/>
-      <c r="F16" s="105"/>
+      <c r="D16" s="131"/>
+      <c r="E16" s="132"/>
+      <c r="F16" s="133"/>
       <c r="G16" s="10"/>
       <c r="H16" s="10" t="s">
         <v>75</v>
@@ -11851,10 +11733,10 @@
       <c r="I16" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="J16" s="139">
+      <c r="J16" s="106">
         <v>6788688.0499999998</v>
       </c>
-      <c r="K16" s="139">
+      <c r="K16" s="106">
         <v>6788688.0499999998</v>
       </c>
       <c r="L16" s="41">
@@ -11869,9 +11751,9 @@
       <c r="O16" s="11"/>
     </row>
     <row r="17" spans="4:15">
-      <c r="D17" s="103"/>
-      <c r="E17" s="104"/>
-      <c r="F17" s="105"/>
+      <c r="D17" s="131"/>
+      <c r="E17" s="132"/>
+      <c r="F17" s="133"/>
       <c r="G17" s="10"/>
       <c r="H17" s="10" t="s">
         <v>76</v>
@@ -11879,10 +11761,10 @@
       <c r="I17" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="J17" s="139">
+      <c r="J17" s="106">
         <v>6689002</v>
       </c>
-      <c r="K17" s="139">
+      <c r="K17" s="106">
         <v>6689002</v>
       </c>
       <c r="L17" s="41">
@@ -11897,9 +11779,9 @@
       <c r="O17" s="11"/>
     </row>
     <row r="18" spans="4:15" ht="14.5" thickBot="1">
-      <c r="D18" s="106"/>
-      <c r="E18" s="107"/>
-      <c r="F18" s="108"/>
+      <c r="D18" s="134"/>
+      <c r="E18" s="135"/>
+      <c r="F18" s="136"/>
       <c r="G18" s="10"/>
       <c r="H18" s="10" t="s">
         <v>77</v>
@@ -11907,10 +11789,10 @@
       <c r="I18" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="J18" s="139">
+      <c r="J18" s="106">
         <v>5776559.9800000004</v>
       </c>
-      <c r="K18" s="139">
+      <c r="K18" s="106">
         <v>5776559.9800000004</v>
       </c>
       <c r="L18" s="41">
@@ -11935,10 +11817,10 @@
       <c r="I19" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="J19" s="139">
+      <c r="J19" s="106">
         <v>3002993.99</v>
       </c>
-      <c r="K19" s="139">
+      <c r="K19" s="106">
         <v>3002993.99</v>
       </c>
       <c r="L19" s="41">
@@ -11961,11 +11843,11 @@
         <v>39</v>
       </c>
       <c r="I20" s="43"/>
-      <c r="J20" s="140">
+      <c r="J20" s="107">
         <f>SUM(J14:J19)</f>
         <v>32046889</v>
       </c>
-      <c r="K20" s="140">
+      <c r="K20" s="107">
         <f>SUM(K14:K19)</f>
         <v>32346889</v>
       </c>
@@ -12063,11 +11945,11 @@
       <c r="O27" s="13"/>
     </row>
     <row r="28" spans="4:15">
-      <c r="D28" s="100" t="s">
+      <c r="D28" s="128" t="s">
         <v>10</v>
       </c>
-      <c r="E28" s="101"/>
-      <c r="F28" s="102"/>
+      <c r="E28" s="129"/>
+      <c r="F28" s="130"/>
       <c r="G28" s="21"/>
       <c r="H28" s="8"/>
       <c r="I28" s="8"/>
@@ -12079,9 +11961,9 @@
       <c r="O28" s="9"/>
     </row>
     <row r="29" spans="4:15">
-      <c r="D29" s="103"/>
-      <c r="E29" s="104"/>
-      <c r="F29" s="105"/>
+      <c r="D29" s="131"/>
+      <c r="E29" s="132"/>
+      <c r="F29" s="133"/>
       <c r="G29" s="22"/>
       <c r="H29" s="50" t="s">
         <v>68</v>
@@ -12095,9 +11977,9 @@
       <c r="O29" s="11"/>
     </row>
     <row r="30" spans="4:15" ht="14.5" thickBot="1">
-      <c r="D30" s="106"/>
-      <c r="E30" s="107"/>
-      <c r="F30" s="108"/>
+      <c r="D30" s="134"/>
+      <c r="E30" s="135"/>
+      <c r="F30" s="136"/>
       <c r="G30" s="10"/>
       <c r="H30" s="50" t="s">
         <v>101</v>
@@ -12111,11 +11993,11 @@
       <c r="O30" s="11"/>
     </row>
     <row r="31" spans="4:15">
-      <c r="D31" s="119" t="s">
+      <c r="D31" s="147" t="s">
         <v>13</v>
       </c>
-      <c r="E31" s="120"/>
-      <c r="F31" s="121"/>
+      <c r="E31" s="148"/>
+      <c r="F31" s="149"/>
       <c r="G31" s="22"/>
       <c r="H31" s="50" t="s">
         <v>69</v>
@@ -12131,9 +12013,9 @@
       <c r="O31" s="11"/>
     </row>
     <row r="32" spans="4:15">
-      <c r="D32" s="122"/>
-      <c r="E32" s="123"/>
-      <c r="F32" s="124"/>
+      <c r="D32" s="150"/>
+      <c r="E32" s="151"/>
+      <c r="F32" s="152"/>
       <c r="G32" s="22"/>
       <c r="H32" s="10"/>
       <c r="I32" s="10"/>
@@ -12145,9 +12027,9 @@
       <c r="O32" s="11"/>
     </row>
     <row r="33" spans="4:15">
-      <c r="D33" s="122"/>
-      <c r="E33" s="123"/>
-      <c r="F33" s="124"/>
+      <c r="D33" s="150"/>
+      <c r="E33" s="151"/>
+      <c r="F33" s="152"/>
       <c r="G33" s="10"/>
       <c r="H33" s="42" t="s">
         <v>40</v>
@@ -12161,9 +12043,9 @@
       <c r="O33" s="11"/>
     </row>
     <row r="34" spans="4:15">
-      <c r="D34" s="122"/>
-      <c r="E34" s="123"/>
-      <c r="F34" s="124"/>
+      <c r="D34" s="150"/>
+      <c r="E34" s="151"/>
+      <c r="F34" s="152"/>
       <c r="G34" s="10"/>
       <c r="H34" s="45" t="s">
         <v>92</v>
@@ -12189,9 +12071,9 @@
       <c r="O34" s="11"/>
     </row>
     <row r="35" spans="4:15" ht="14.5" thickBot="1">
-      <c r="D35" s="125"/>
-      <c r="E35" s="126"/>
-      <c r="F35" s="127"/>
+      <c r="D35" s="153"/>
+      <c r="E35" s="154"/>
+      <c r="F35" s="155"/>
       <c r="G35" s="10"/>
       <c r="H35" s="10" t="s">
         <v>88</v>
@@ -12219,11 +12101,11 @@
       <c r="O35" s="11"/>
     </row>
     <row r="36" spans="4:15">
-      <c r="D36" s="100" t="s">
+      <c r="D36" s="128" t="s">
         <v>67</v>
       </c>
-      <c r="E36" s="101"/>
-      <c r="F36" s="102"/>
+      <c r="E36" s="129"/>
+      <c r="F36" s="130"/>
       <c r="G36" s="10"/>
       <c r="H36" s="10" t="s">
         <v>91</v>
@@ -12251,9 +12133,9 @@
       <c r="O36" s="11"/>
     </row>
     <row r="37" spans="4:15" ht="14.5" thickBot="1">
-      <c r="D37" s="103"/>
-      <c r="E37" s="104"/>
-      <c r="F37" s="105"/>
+      <c r="D37" s="131"/>
+      <c r="E37" s="132"/>
+      <c r="F37" s="133"/>
       <c r="G37" s="10"/>
       <c r="H37" s="46" t="s">
         <v>39</v>
@@ -12276,9 +12158,9 @@
       <c r="O37" s="11"/>
     </row>
     <row r="38" spans="4:15">
-      <c r="D38" s="103"/>
-      <c r="E38" s="104"/>
-      <c r="F38" s="105"/>
+      <c r="D38" s="131"/>
+      <c r="E38" s="132"/>
+      <c r="F38" s="133"/>
       <c r="G38" s="10"/>
       <c r="H38" s="10"/>
       <c r="I38" s="10"/>
@@ -12290,9 +12172,9 @@
       <c r="O38" s="11"/>
     </row>
     <row r="39" spans="4:15" ht="14.5" thickBot="1">
-      <c r="D39" s="106"/>
-      <c r="E39" s="107"/>
-      <c r="F39" s="108"/>
+      <c r="D39" s="134"/>
+      <c r="E39" s="135"/>
+      <c r="F39" s="136"/>
       <c r="G39" s="10"/>
       <c r="H39" s="42" t="s">
         <v>41</v>
@@ -12839,11 +12721,11 @@
       <c r="Q8" s="13"/>
     </row>
     <row r="9" spans="4:17">
-      <c r="D9" s="100" t="s">
+      <c r="D9" s="128" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="101"/>
-      <c r="F9" s="102"/>
+      <c r="E9" s="129"/>
+      <c r="F9" s="130"/>
       <c r="G9" s="21"/>
       <c r="H9" s="8"/>
       <c r="I9" s="8"/>
@@ -12857,9 +12739,9 @@
       <c r="Q9" s="9"/>
     </row>
     <row r="10" spans="4:17" ht="14.5" thickBot="1">
-      <c r="D10" s="103"/>
-      <c r="E10" s="104"/>
-      <c r="F10" s="105"/>
+      <c r="D10" s="131"/>
+      <c r="E10" s="132"/>
+      <c r="F10" s="133"/>
       <c r="G10" s="22"/>
       <c r="H10" s="22"/>
       <c r="I10" s="22"/>
@@ -12873,9 +12755,9 @@
       <c r="Q10" s="11"/>
     </row>
     <row r="11" spans="4:17" ht="14.5" thickBot="1">
-      <c r="D11" s="106"/>
-      <c r="E11" s="107"/>
-      <c r="F11" s="108"/>
+      <c r="D11" s="134"/>
+      <c r="E11" s="135"/>
+      <c r="F11" s="136"/>
       <c r="G11" s="10"/>
       <c r="H11" s="70" t="s">
         <v>107</v>
@@ -12897,11 +12779,11 @@
       <c r="Q11" s="11"/>
     </row>
     <row r="12" spans="4:17" ht="14.5" thickBot="1">
-      <c r="D12" s="100" t="s">
+      <c r="D12" s="128" t="s">
         <v>13</v>
       </c>
-      <c r="E12" s="101"/>
-      <c r="F12" s="102"/>
+      <c r="E12" s="129"/>
+      <c r="F12" s="130"/>
       <c r="G12" s="22"/>
       <c r="H12" s="79"/>
       <c r="I12" s="68"/>
@@ -12915,9 +12797,9 @@
       <c r="Q12" s="11"/>
     </row>
     <row r="13" spans="4:17" ht="14.5" thickBot="1">
-      <c r="D13" s="103"/>
-      <c r="E13" s="104"/>
-      <c r="F13" s="105"/>
+      <c r="D13" s="131"/>
+      <c r="E13" s="132"/>
+      <c r="F13" s="133"/>
       <c r="G13" s="22"/>
       <c r="H13" s="78" t="s">
         <v>131</v>
@@ -12929,19 +12811,19 @@
       <c r="K13" s="10"/>
       <c r="L13" s="11"/>
       <c r="M13" s="10"/>
-      <c r="N13" s="135" t="s">
+      <c r="N13" s="102" t="s">
         <v>116</v>
       </c>
-      <c r="O13" s="138"/>
+      <c r="O13" s="105"/>
       <c r="P13" s="91" t="s">
         <v>137</v>
       </c>
       <c r="Q13" s="11"/>
     </row>
     <row r="14" spans="4:17" ht="14.5" thickBot="1">
-      <c r="D14" s="103"/>
-      <c r="E14" s="104"/>
-      <c r="F14" s="105"/>
+      <c r="D14" s="131"/>
+      <c r="E14" s="132"/>
+      <c r="F14" s="133"/>
       <c r="G14" s="22"/>
       <c r="H14" s="77" t="s">
         <v>109</v>
@@ -12953,19 +12835,19 @@
       <c r="K14" s="10"/>
       <c r="L14" s="11"/>
       <c r="M14" s="10"/>
-      <c r="N14" s="136" t="s">
+      <c r="N14" s="103" t="s">
         <v>117</v>
       </c>
-      <c r="O14" s="137"/>
+      <c r="O14" s="104"/>
       <c r="P14" s="92" t="s">
         <v>138</v>
       </c>
       <c r="Q14" s="11"/>
     </row>
     <row r="15" spans="4:17" ht="14.5" thickBot="1">
-      <c r="D15" s="103"/>
-      <c r="E15" s="104"/>
-      <c r="F15" s="105"/>
+      <c r="D15" s="131"/>
+      <c r="E15" s="132"/>
+      <c r="F15" s="133"/>
       <c r="G15" s="10"/>
       <c r="H15" s="77" t="s">
         <v>110</v>
@@ -12977,19 +12859,19 @@
       <c r="K15" s="56"/>
       <c r="L15" s="59"/>
       <c r="M15" s="56"/>
-      <c r="N15" s="133" t="s">
+      <c r="N15" s="100" t="s">
         <v>123</v>
       </c>
-      <c r="O15" s="134"/>
+      <c r="O15" s="101"/>
       <c r="P15" s="93" t="s">
         <v>139</v>
       </c>
       <c r="Q15" s="11"/>
     </row>
     <row r="16" spans="4:17" ht="14.5" thickBot="1">
-      <c r="D16" s="106"/>
-      <c r="E16" s="107"/>
-      <c r="F16" s="108"/>
+      <c r="D16" s="134"/>
+      <c r="E16" s="135"/>
+      <c r="F16" s="136"/>
       <c r="G16" s="10"/>
       <c r="H16" s="77" t="s">
         <v>115</v>
@@ -13007,11 +12889,11 @@
       <c r="Q16" s="11"/>
     </row>
     <row r="17" spans="4:17">
-      <c r="D17" s="128" t="s">
+      <c r="D17" s="156" t="s">
         <v>105</v>
       </c>
-      <c r="E17" s="120"/>
-      <c r="F17" s="121"/>
+      <c r="E17" s="148"/>
+      <c r="F17" s="149"/>
       <c r="G17" s="10"/>
       <c r="H17" s="77" t="s">
         <v>111</v>
@@ -13029,9 +12911,9 @@
       <c r="Q17" s="11"/>
     </row>
     <row r="18" spans="4:17">
-      <c r="D18" s="122"/>
-      <c r="E18" s="123"/>
-      <c r="F18" s="124"/>
+      <c r="D18" s="150"/>
+      <c r="E18" s="151"/>
+      <c r="F18" s="152"/>
       <c r="G18" s="10"/>
       <c r="H18" s="77" t="s">
         <v>112</v>
@@ -13049,9 +12931,9 @@
       <c r="Q18" s="11"/>
     </row>
     <row r="19" spans="4:17">
-      <c r="D19" s="122"/>
-      <c r="E19" s="123"/>
-      <c r="F19" s="124"/>
+      <c r="D19" s="150"/>
+      <c r="E19" s="151"/>
+      <c r="F19" s="152"/>
       <c r="G19" s="10"/>
       <c r="H19" s="77" t="s">
         <v>132</v>
@@ -13069,9 +12951,9 @@
       <c r="Q19" s="11"/>
     </row>
     <row r="20" spans="4:17" ht="14.5" thickBot="1">
-      <c r="D20" s="125"/>
-      <c r="E20" s="126"/>
-      <c r="F20" s="127"/>
+      <c r="D20" s="153"/>
+      <c r="E20" s="154"/>
+      <c r="F20" s="155"/>
       <c r="G20" s="10"/>
       <c r="H20" s="57"/>
       <c r="I20" s="40"/>
@@ -13399,11 +13281,11 @@
       <c r="Q8" s="13"/>
     </row>
     <row r="9" spans="4:17">
-      <c r="D9" s="100" t="s">
+      <c r="D9" s="128" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="101"/>
-      <c r="F9" s="102"/>
+      <c r="E9" s="129"/>
+      <c r="F9" s="130"/>
       <c r="G9" s="21"/>
       <c r="H9" s="8"/>
       <c r="I9" s="8"/>
@@ -13417,9 +13299,9 @@
       <c r="Q9" s="9"/>
     </row>
     <row r="10" spans="4:17">
-      <c r="D10" s="103"/>
-      <c r="E10" s="104"/>
-      <c r="F10" s="105"/>
+      <c r="D10" s="131"/>
+      <c r="E10" s="132"/>
+      <c r="F10" s="133"/>
       <c r="G10" s="22"/>
       <c r="H10" s="22"/>
       <c r="I10" s="22"/>
@@ -13433,9 +13315,9 @@
       <c r="Q10" s="11"/>
     </row>
     <row r="11" spans="4:17" ht="14.5" thickBot="1">
-      <c r="D11" s="106"/>
-      <c r="E11" s="107"/>
-      <c r="F11" s="108"/>
+      <c r="D11" s="134"/>
+      <c r="E11" s="135"/>
+      <c r="F11" s="136"/>
       <c r="G11" s="10"/>
       <c r="H11" s="10"/>
       <c r="I11" s="10"/>
@@ -13449,11 +13331,11 @@
       <c r="Q11" s="11"/>
     </row>
     <row r="12" spans="4:17" ht="14.5" thickBot="1">
-      <c r="D12" s="100" t="s">
+      <c r="D12" s="128" t="s">
         <v>13</v>
       </c>
-      <c r="E12" s="101"/>
-      <c r="F12" s="102"/>
+      <c r="E12" s="129"/>
+      <c r="F12" s="130"/>
       <c r="G12" s="22"/>
       <c r="H12" s="22"/>
       <c r="I12" s="22"/>
@@ -13467,27 +13349,27 @@
       <c r="Q12" s="11"/>
     </row>
     <row r="13" spans="4:17">
-      <c r="D13" s="103"/>
-      <c r="E13" s="104"/>
-      <c r="F13" s="105"/>
+      <c r="D13" s="131"/>
+      <c r="E13" s="132"/>
+      <c r="F13" s="133"/>
       <c r="G13" s="22"/>
-      <c r="H13" s="129" t="s">
+      <c r="H13" s="157" t="s">
         <v>125</v>
       </c>
-      <c r="I13" s="130"/>
-      <c r="J13" s="144"/>
-      <c r="K13" s="144"/>
-      <c r="L13" s="144"/>
-      <c r="M13" s="144"/>
-      <c r="N13" s="144"/>
-      <c r="O13" s="144"/>
+      <c r="I13" s="158"/>
+      <c r="J13" s="159"/>
+      <c r="K13" s="159"/>
+      <c r="L13" s="159"/>
+      <c r="M13" s="159"/>
+      <c r="N13" s="159"/>
+      <c r="O13" s="159"/>
       <c r="P13" s="10"/>
       <c r="Q13" s="11"/>
     </row>
     <row r="14" spans="4:17">
-      <c r="D14" s="103"/>
-      <c r="E14" s="104"/>
-      <c r="F14" s="105"/>
+      <c r="D14" s="131"/>
+      <c r="E14" s="132"/>
+      <c r="F14" s="133"/>
       <c r="G14" s="22"/>
       <c r="H14" s="63"/>
       <c r="I14" s="74"/>
@@ -13501,9 +13383,9 @@
       <c r="Q14" s="11"/>
     </row>
     <row r="15" spans="4:17">
-      <c r="D15" s="103"/>
-      <c r="E15" s="104"/>
-      <c r="F15" s="105"/>
+      <c r="D15" s="131"/>
+      <c r="E15" s="132"/>
+      <c r="F15" s="133"/>
       <c r="G15" s="10"/>
       <c r="H15" s="63"/>
       <c r="I15" s="59"/>
@@ -13517,9 +13399,9 @@
       <c r="Q15" s="11"/>
     </row>
     <row r="16" spans="4:17" ht="14.5" thickBot="1">
-      <c r="D16" s="106"/>
-      <c r="E16" s="107"/>
-      <c r="F16" s="108"/>
+      <c r="D16" s="134"/>
+      <c r="E16" s="135"/>
+      <c r="F16" s="136"/>
       <c r="G16" s="10"/>
       <c r="H16" s="63"/>
       <c r="I16" s="11"/>
@@ -13533,11 +13415,11 @@
       <c r="Q16" s="11"/>
     </row>
     <row r="17" spans="4:17">
-      <c r="D17" s="128" t="s">
+      <c r="D17" s="156" t="s">
         <v>124</v>
       </c>
-      <c r="E17" s="120"/>
-      <c r="F17" s="121"/>
+      <c r="E17" s="148"/>
+      <c r="F17" s="149"/>
       <c r="G17" s="10"/>
       <c r="H17" s="63"/>
       <c r="I17" s="11"/>
@@ -13551,9 +13433,9 @@
       <c r="Q17" s="11"/>
     </row>
     <row r="18" spans="4:17">
-      <c r="D18" s="122"/>
-      <c r="E18" s="123"/>
-      <c r="F18" s="124"/>
+      <c r="D18" s="150"/>
+      <c r="E18" s="151"/>
+      <c r="F18" s="152"/>
       <c r="G18" s="10"/>
       <c r="H18" s="63"/>
       <c r="I18" s="11"/>
@@ -13567,9 +13449,9 @@
       <c r="Q18" s="11"/>
     </row>
     <row r="19" spans="4:17">
-      <c r="D19" s="122"/>
-      <c r="E19" s="123"/>
-      <c r="F19" s="124"/>
+      <c r="D19" s="150"/>
+      <c r="E19" s="151"/>
+      <c r="F19" s="152"/>
       <c r="G19" s="10"/>
       <c r="H19" s="14"/>
       <c r="I19" s="11"/>
@@ -13583,9 +13465,9 @@
       <c r="Q19" s="11"/>
     </row>
     <row r="20" spans="4:17" ht="14.5" thickBot="1">
-      <c r="D20" s="125"/>
-      <c r="E20" s="126"/>
-      <c r="F20" s="127"/>
+      <c r="D20" s="153"/>
+      <c r="E20" s="154"/>
+      <c r="F20" s="155"/>
       <c r="G20" s="10"/>
       <c r="H20" s="57"/>
       <c r="I20" s="74"/>
@@ -13731,10 +13613,10 @@
       <c r="E29" s="10"/>
       <c r="F29" s="11"/>
       <c r="G29" s="10"/>
-      <c r="H29" s="150" t="s">
+      <c r="H29" s="114" t="s">
         <v>126</v>
       </c>
-      <c r="I29" s="151"/>
+      <c r="I29" s="115"/>
       <c r="J29" s="40"/>
       <c r="K29" s="10"/>
       <c r="L29" s="10"/>
@@ -13749,16 +13631,16 @@
       <c r="E30" s="10"/>
       <c r="F30" s="11"/>
       <c r="G30" s="10"/>
-      <c r="H30" s="131" t="s">
+      <c r="H30" s="160" t="s">
         <v>125</v>
       </c>
-      <c r="I30" s="132"/>
-      <c r="J30" s="145"/>
-      <c r="K30" s="145"/>
-      <c r="L30" s="145"/>
-      <c r="M30" s="145"/>
-      <c r="N30" s="145"/>
-      <c r="O30" s="145"/>
+      <c r="I30" s="161"/>
+      <c r="J30" s="162"/>
+      <c r="K30" s="162"/>
+      <c r="L30" s="162"/>
+      <c r="M30" s="162"/>
+      <c r="N30" s="162"/>
+      <c r="O30" s="162"/>
       <c r="P30" s="22"/>
       <c r="Q30" s="11"/>
     </row>
@@ -13790,7 +13672,7 @@
       <c r="H32" s="96" t="s">
         <v>127</v>
       </c>
-      <c r="I32" s="152">
+      <c r="I32" s="116">
         <v>40</v>
       </c>
       <c r="J32" s="40"/>
@@ -13810,7 +13692,7 @@
       <c r="H33" s="94" t="s">
         <v>140</v>
       </c>
-      <c r="I33" s="153">
+      <c r="I33" s="117">
         <v>40.5</v>
       </c>
       <c r="J33" s="40"/>
@@ -13830,7 +13712,7 @@
       <c r="H34" s="94" t="s">
         <v>141</v>
       </c>
-      <c r="I34" s="153">
+      <c r="I34" s="117">
         <v>39.6</v>
       </c>
       <c r="J34" s="51"/>
@@ -13850,7 +13732,7 @@
       <c r="H35" s="99" t="s">
         <v>142</v>
       </c>
-      <c r="I35" s="154">
+      <c r="I35" s="118">
         <v>41</v>
       </c>
       <c r="J35" s="51"/>
@@ -13928,17 +13810,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="D9:F11"/>
-    <mergeCell ref="D12:F16"/>
-    <mergeCell ref="D17:F20"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="J13:K13"/>
     <mergeCell ref="N13:O13"/>
     <mergeCell ref="H30:I30"/>
     <mergeCell ref="J30:K30"/>
     <mergeCell ref="L30:M30"/>
     <mergeCell ref="N30:O30"/>
     <mergeCell ref="L13:M13"/>
+    <mergeCell ref="D9:F11"/>
+    <mergeCell ref="D12:F16"/>
+    <mergeCell ref="D17:F20"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="J13:K13"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -13950,8 +13832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F50A82F-4F20-458B-9395-69DAEEAD96DD}">
   <dimension ref="E4:U38"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Y4" sqref="Y4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -13974,7 +13856,7 @@
       <c r="M5" s="3"/>
       <c r="N5" s="3"/>
       <c r="O5" s="8"/>
-      <c r="P5" s="146"/>
+      <c r="P5" s="110"/>
       <c r="Q5" s="3"/>
       <c r="R5" s="3"/>
       <c r="S5" s="3" t="s">
@@ -13997,7 +13879,7 @@
       <c r="M6" s="5"/>
       <c r="N6" s="5"/>
       <c r="O6" s="10"/>
-      <c r="P6" s="147"/>
+      <c r="P6" s="111"/>
       <c r="Q6" s="5"/>
       <c r="R6" s="5"/>
       <c r="S6" s="5" t="s">
@@ -14026,11 +13908,11 @@
       <c r="U7" s="13"/>
     </row>
     <row r="8" spans="5:21" ht="14" customHeight="1">
-      <c r="E8" s="128" t="s">
+      <c r="E8" s="156" t="s">
         <v>151</v>
       </c>
-      <c r="F8" s="120"/>
-      <c r="G8" s="121"/>
+      <c r="F8" s="148"/>
+      <c r="G8" s="149"/>
       <c r="H8" s="21"/>
       <c r="I8" s="21"/>
       <c r="J8" s="8"/>
@@ -14047,9 +13929,9 @@
       <c r="U8" s="9"/>
     </row>
     <row r="9" spans="5:21">
-      <c r="E9" s="122"/>
-      <c r="F9" s="123"/>
-      <c r="G9" s="124"/>
+      <c r="E9" s="150"/>
+      <c r="F9" s="151"/>
+      <c r="G9" s="152"/>
       <c r="H9" s="22"/>
       <c r="I9" s="22"/>
       <c r="J9" s="22"/>
@@ -14066,9 +13948,9 @@
       <c r="U9" s="11"/>
     </row>
     <row r="10" spans="5:21" ht="14.5" thickBot="1">
-      <c r="E10" s="122"/>
-      <c r="F10" s="123"/>
-      <c r="G10" s="124"/>
+      <c r="E10" s="150"/>
+      <c r="F10" s="151"/>
+      <c r="G10" s="152"/>
       <c r="H10" s="10"/>
       <c r="I10" s="10"/>
       <c r="J10" s="10"/>
@@ -14085,11 +13967,11 @@
       <c r="U10" s="11"/>
     </row>
     <row r="11" spans="5:21">
-      <c r="E11" s="100" t="s">
+      <c r="E11" s="128" t="s">
         <v>3</v>
       </c>
-      <c r="F11" s="101"/>
-      <c r="G11" s="102"/>
+      <c r="F11" s="129"/>
+      <c r="G11" s="130"/>
       <c r="H11" s="22"/>
       <c r="I11" s="22"/>
       <c r="J11" s="22"/>
@@ -14106,31 +13988,31 @@
       <c r="U11" s="11"/>
     </row>
     <row r="12" spans="5:21">
-      <c r="E12" s="103"/>
-      <c r="F12" s="104"/>
-      <c r="G12" s="105"/>
+      <c r="E12" s="131"/>
+      <c r="F12" s="132"/>
+      <c r="G12" s="133"/>
       <c r="H12" s="22"/>
       <c r="I12" s="22"/>
-      <c r="J12" s="144"/>
-      <c r="K12" s="144"/>
-      <c r="L12" s="144"/>
-      <c r="M12" s="144"/>
-      <c r="N12" s="144"/>
-      <c r="O12" s="144"/>
-      <c r="P12" s="144"/>
-      <c r="Q12" s="144"/>
+      <c r="J12" s="159"/>
+      <c r="K12" s="159"/>
+      <c r="L12" s="159"/>
+      <c r="M12" s="159"/>
+      <c r="N12" s="159"/>
+      <c r="O12" s="159"/>
+      <c r="P12" s="159"/>
+      <c r="Q12" s="159"/>
       <c r="R12" s="10"/>
       <c r="S12" s="10"/>
       <c r="T12" s="10"/>
       <c r="U12" s="11"/>
     </row>
     <row r="13" spans="5:21">
-      <c r="E13" s="103"/>
-      <c r="F13" s="104"/>
-      <c r="G13" s="105"/>
+      <c r="E13" s="131"/>
+      <c r="F13" s="132"/>
+      <c r="G13" s="133"/>
       <c r="H13" s="22"/>
       <c r="I13" s="22"/>
-      <c r="J13" s="143"/>
+      <c r="J13" s="109"/>
       <c r="K13" s="40"/>
       <c r="L13" s="40"/>
       <c r="M13" s="10"/>
@@ -14144,12 +14026,12 @@
       <c r="U13" s="11"/>
     </row>
     <row r="14" spans="5:21">
-      <c r="E14" s="103"/>
-      <c r="F14" s="104"/>
-      <c r="G14" s="105"/>
+      <c r="E14" s="131"/>
+      <c r="F14" s="132"/>
+      <c r="G14" s="133"/>
       <c r="H14" s="10"/>
       <c r="I14" s="10"/>
-      <c r="J14" s="143"/>
+      <c r="J14" s="109"/>
       <c r="K14" s="56"/>
       <c r="L14" s="56"/>
       <c r="M14" s="56"/>
@@ -14163,12 +14045,12 @@
       <c r="U14" s="11"/>
     </row>
     <row r="15" spans="5:21" ht="14.5" thickBot="1">
-      <c r="E15" s="106"/>
-      <c r="F15" s="107"/>
-      <c r="G15" s="108"/>
+      <c r="E15" s="134"/>
+      <c r="F15" s="135"/>
+      <c r="G15" s="136"/>
       <c r="H15" s="10"/>
       <c r="I15" s="10"/>
-      <c r="J15" s="143"/>
+      <c r="J15" s="109"/>
       <c r="K15" s="10"/>
       <c r="L15" s="10"/>
       <c r="M15" s="10"/>
@@ -14182,14 +14064,14 @@
       <c r="U15" s="11"/>
     </row>
     <row r="16" spans="5:21">
-      <c r="E16" s="142" t="s">
+      <c r="E16" s="163" t="s">
         <v>34</v>
       </c>
-      <c r="F16" s="101"/>
-      <c r="G16" s="102"/>
+      <c r="F16" s="129"/>
+      <c r="G16" s="130"/>
       <c r="H16" s="10"/>
       <c r="I16" s="10"/>
-      <c r="J16" s="143"/>
+      <c r="J16" s="109"/>
       <c r="K16" s="10"/>
       <c r="L16" s="10"/>
       <c r="M16" s="10"/>
@@ -14203,12 +14085,12 @@
       <c r="U16" s="11"/>
     </row>
     <row r="17" spans="5:21">
-      <c r="E17" s="103"/>
-      <c r="F17" s="104"/>
-      <c r="G17" s="105"/>
+      <c r="E17" s="131"/>
+      <c r="F17" s="132"/>
+      <c r="G17" s="133"/>
       <c r="H17" s="10"/>
       <c r="I17" s="10"/>
-      <c r="J17" s="143"/>
+      <c r="J17" s="109"/>
       <c r="K17" s="10"/>
       <c r="L17" s="10"/>
       <c r="M17" s="10"/>
@@ -14222,9 +14104,9 @@
       <c r="U17" s="11"/>
     </row>
     <row r="18" spans="5:21">
-      <c r="E18" s="103"/>
-      <c r="F18" s="104"/>
-      <c r="G18" s="105"/>
+      <c r="E18" s="131"/>
+      <c r="F18" s="132"/>
+      <c r="G18" s="133"/>
       <c r="H18" s="10"/>
       <c r="I18" s="10"/>
       <c r="J18" s="10"/>
@@ -14241,9 +14123,9 @@
       <c r="U18" s="11"/>
     </row>
     <row r="19" spans="5:21" ht="14.5" thickBot="1">
-      <c r="E19" s="106"/>
-      <c r="F19" s="107"/>
-      <c r="G19" s="108"/>
+      <c r="E19" s="134"/>
+      <c r="F19" s="135"/>
+      <c r="G19" s="136"/>
       <c r="H19" s="10"/>
       <c r="I19" s="10"/>
       <c r="J19" s="40"/>
@@ -14436,14 +14318,14 @@
       <c r="G29" s="11"/>
       <c r="H29" s="10"/>
       <c r="I29" s="10"/>
-      <c r="J29" s="145"/>
-      <c r="K29" s="145"/>
-      <c r="L29" s="145"/>
-      <c r="M29" s="145"/>
-      <c r="N29" s="145"/>
-      <c r="O29" s="145"/>
-      <c r="P29" s="145"/>
-      <c r="Q29" s="145"/>
+      <c r="J29" s="162"/>
+      <c r="K29" s="162"/>
+      <c r="L29" s="162"/>
+      <c r="M29" s="162"/>
+      <c r="N29" s="162"/>
+      <c r="O29" s="162"/>
+      <c r="P29" s="162"/>
+      <c r="Q29" s="162"/>
       <c r="R29" s="22"/>
       <c r="S29" s="22"/>
       <c r="T29" s="22"/>
@@ -14622,17 +14504,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="P12:Q12"/>
+    <mergeCell ref="E8:G10"/>
+    <mergeCell ref="E11:G15"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="L12:M12"/>
+    <mergeCell ref="N12:O12"/>
     <mergeCell ref="E16:G19"/>
     <mergeCell ref="J29:K29"/>
     <mergeCell ref="L29:M29"/>
     <mergeCell ref="N29:O29"/>
     <mergeCell ref="P29:Q29"/>
-    <mergeCell ref="E8:G10"/>
-    <mergeCell ref="E11:G15"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="L12:M12"/>
-    <mergeCell ref="N12:O12"/>
-    <mergeCell ref="P12:Q12"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -14711,11 +14593,11 @@
       <c r="S7" s="13"/>
     </row>
     <row r="8" spans="6:19">
-      <c r="F8" s="100" t="s">
+      <c r="F8" s="128" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="101"/>
-      <c r="H8" s="102"/>
+      <c r="G8" s="129"/>
+      <c r="H8" s="130"/>
       <c r="I8" s="21"/>
       <c r="J8" s="8"/>
       <c r="K8" s="8"/>
@@ -14729,9 +14611,9 @@
       <c r="S8" s="9"/>
     </row>
     <row r="9" spans="6:19">
-      <c r="F9" s="103"/>
-      <c r="G9" s="104"/>
-      <c r="H9" s="105"/>
+      <c r="F9" s="131"/>
+      <c r="G9" s="132"/>
+      <c r="H9" s="133"/>
       <c r="I9" s="22"/>
       <c r="J9" s="22"/>
       <c r="K9" s="22"/>
@@ -14745,9 +14627,9 @@
       <c r="S9" s="11"/>
     </row>
     <row r="10" spans="6:19" ht="14.5" thickBot="1">
-      <c r="F10" s="106"/>
-      <c r="G10" s="107"/>
-      <c r="H10" s="108"/>
+      <c r="F10" s="134"/>
+      <c r="G10" s="135"/>
+      <c r="H10" s="136"/>
       <c r="I10" s="10"/>
       <c r="J10" s="10"/>
       <c r="K10" s="10"/>
@@ -14761,11 +14643,11 @@
       <c r="S10" s="11"/>
     </row>
     <row r="11" spans="6:19">
-      <c r="F11" s="100" t="s">
+      <c r="F11" s="128" t="s">
         <v>13</v>
       </c>
-      <c r="G11" s="101"/>
-      <c r="H11" s="102"/>
+      <c r="G11" s="129"/>
+      <c r="H11" s="130"/>
       <c r="I11" s="22"/>
       <c r="J11" s="22"/>
       <c r="K11" s="22"/>
@@ -14779,11 +14661,11 @@
       <c r="S11" s="11"/>
     </row>
     <row r="12" spans="6:19">
-      <c r="F12" s="103"/>
-      <c r="G12" s="104"/>
-      <c r="H12" s="105"/>
+      <c r="F12" s="131"/>
+      <c r="G12" s="132"/>
+      <c r="H12" s="133"/>
       <c r="I12" s="22"/>
-      <c r="J12" s="143"/>
+      <c r="J12" s="109"/>
       <c r="K12" s="86"/>
       <c r="L12" s="10"/>
       <c r="M12" s="10"/>
@@ -14795,11 +14677,11 @@
       <c r="S12" s="11"/>
     </row>
     <row r="13" spans="6:19">
-      <c r="F13" s="103"/>
-      <c r="G13" s="104"/>
-      <c r="H13" s="105"/>
+      <c r="F13" s="131"/>
+      <c r="G13" s="132"/>
+      <c r="H13" s="133"/>
       <c r="I13" s="22"/>
-      <c r="J13" s="143"/>
+      <c r="J13" s="109"/>
       <c r="K13" s="87"/>
       <c r="L13" s="40"/>
       <c r="M13" s="10"/>
@@ -14811,11 +14693,11 @@
       <c r="S13" s="11"/>
     </row>
     <row r="14" spans="6:19">
-      <c r="F14" s="103"/>
-      <c r="G14" s="104"/>
-      <c r="H14" s="105"/>
+      <c r="F14" s="131"/>
+      <c r="G14" s="132"/>
+      <c r="H14" s="133"/>
       <c r="I14" s="10"/>
-      <c r="J14" s="143"/>
+      <c r="J14" s="109"/>
       <c r="K14" s="87"/>
       <c r="L14" s="56"/>
       <c r="M14" s="56"/>
@@ -14823,15 +14705,15 @@
       <c r="O14" s="56"/>
       <c r="P14" s="10"/>
       <c r="Q14" s="56"/>
-      <c r="R14" s="148"/>
+      <c r="R14" s="112"/>
       <c r="S14" s="11"/>
     </row>
     <row r="15" spans="6:19" ht="14.5" thickBot="1">
-      <c r="F15" s="106"/>
-      <c r="G15" s="107"/>
-      <c r="H15" s="108"/>
+      <c r="F15" s="134"/>
+      <c r="G15" s="135"/>
+      <c r="H15" s="136"/>
       <c r="I15" s="10"/>
-      <c r="J15" s="143"/>
+      <c r="J15" s="109"/>
       <c r="K15" s="88"/>
       <c r="L15" s="10"/>
       <c r="M15" s="10"/>
@@ -14843,13 +14725,13 @@
       <c r="S15" s="11"/>
     </row>
     <row r="16" spans="6:19">
-      <c r="F16" s="142" t="s">
+      <c r="F16" s="163" t="s">
         <v>105</v>
       </c>
-      <c r="G16" s="101"/>
-      <c r="H16" s="102"/>
+      <c r="G16" s="129"/>
+      <c r="H16" s="130"/>
       <c r="I16" s="10"/>
-      <c r="J16" s="143"/>
+      <c r="J16" s="109"/>
       <c r="K16" s="88"/>
       <c r="L16" s="10"/>
       <c r="M16" s="10"/>
@@ -14861,11 +14743,11 @@
       <c r="S16" s="11"/>
     </row>
     <row r="17" spans="6:19">
-      <c r="F17" s="103"/>
-      <c r="G17" s="104"/>
-      <c r="H17" s="105"/>
+      <c r="F17" s="131"/>
+      <c r="G17" s="132"/>
+      <c r="H17" s="133"/>
       <c r="I17" s="10"/>
-      <c r="J17" s="143"/>
+      <c r="J17" s="109"/>
       <c r="K17" s="88"/>
       <c r="L17" s="10"/>
       <c r="M17" s="10"/>
@@ -14877,11 +14759,11 @@
       <c r="S17" s="11"/>
     </row>
     <row r="18" spans="6:19">
-      <c r="F18" s="103"/>
-      <c r="G18" s="104"/>
-      <c r="H18" s="105"/>
+      <c r="F18" s="131"/>
+      <c r="G18" s="132"/>
+      <c r="H18" s="133"/>
       <c r="I18" s="10"/>
-      <c r="J18" s="143"/>
+      <c r="J18" s="109"/>
       <c r="K18" s="88"/>
       <c r="L18" s="10"/>
       <c r="M18" s="10"/>
@@ -14893,9 +14775,9 @@
       <c r="S18" s="11"/>
     </row>
     <row r="19" spans="6:19" ht="14.5" thickBot="1">
-      <c r="F19" s="106"/>
-      <c r="G19" s="107"/>
-      <c r="H19" s="108"/>
+      <c r="F19" s="134"/>
+      <c r="G19" s="135"/>
+      <c r="H19" s="136"/>
       <c r="I19" s="10"/>
       <c r="J19" s="40"/>
       <c r="K19" s="40"/>
@@ -14993,11 +14875,11 @@
       <c r="G25" s="10"/>
       <c r="H25" s="11"/>
       <c r="I25" s="10"/>
-      <c r="J25" s="149"/>
-      <c r="K25" s="149"/>
-      <c r="L25" s="149"/>
-      <c r="M25" s="149"/>
-      <c r="N25" s="149"/>
+      <c r="J25" s="113"/>
+      <c r="K25" s="113"/>
+      <c r="L25" s="113"/>
+      <c r="M25" s="113"/>
+      <c r="N25" s="113"/>
       <c r="O25" s="10"/>
       <c r="P25" s="10"/>
       <c r="Q25" s="22"/>

</xml_diff>